<commit_message>
BTP 2019-12-01 1.05% inserted
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/EUR_ITALY.xlsx
+++ b/QuantLibXL/Data2/XLS/EUR_ITALY.xlsx
@@ -1568,7 +1568,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="26">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1801,28 +1801,6 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -1867,7 +1845,7 @@
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="140">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="4" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
@@ -2074,30 +2052,19 @@
     <xf numFmtId="0" fontId="9" fillId="4" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="13" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="9" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="9" fillId="0" borderId="24" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="24" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="24" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="9" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="22" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="22" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="20" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="4" borderId="11" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="16" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2514,12 +2481,12 @@
     </row>
     <row r="2" spans="1:5" s="4" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
-      <c r="B2" s="144" t="s">
+      <c r="B2" s="137" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="145"/>
-      <c r="D2" s="145"/>
-      <c r="E2" s="146"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="139"/>
     </row>
     <row r="3" spans="1:5" s="4" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
@@ -4560,10 +4527,10 @@
   <dimension ref="A1:R97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="8" ySplit="7" topLeftCell="I8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="8" ySplit="7" topLeftCell="I32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" outlineLevelCol="1" x14ac:dyDescent="0.2"/>
@@ -4647,7 +4614,7 @@
     <row r="4" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="62"/>
       <c r="B4" s="21" t="str">
-        <f>IF(Serialize,_xll.ohObjectSave(I9:I97,SerializationPath&amp;FileName,FileOverwrite,Serialize),"---")</f>
+        <f>IF(Serialize,_xll.ohObjectSave(I8:I97,SerializationPath&amp;FileName,FileOverwrite,Serialize),"---")</f>
         <v>---</v>
       </c>
       <c r="C4" s="25" t="s">
@@ -4694,8 +4661,8 @@
       <c r="G6" s="22"/>
       <c r="H6" s="22"/>
       <c r="I6" s="50">
-        <f>_xll.qlBondSettlementDate(I9,)</f>
-        <v>42017</v>
+        <f>_xll.qlBondSettlementDate(I8,)</f>
+        <v>42018</v>
       </c>
       <c r="J6" s="22"/>
       <c r="K6" s="22"/>
@@ -4747,32 +4714,32 @@
         <f>_xll.ohRangeRetrieveError(I8)</f>
         <v/>
       </c>
-      <c r="C8" s="123" t="s">
-        <v>453</v>
-      </c>
-      <c r="D8" s="124">
-        <v>43800</v>
-      </c>
-      <c r="E8" s="125">
-        <v>1.0500000000000001E-2</v>
-      </c>
-      <c r="F8" s="126">
-        <v>100</v>
-      </c>
-      <c r="G8" s="124">
-        <v>41974</v>
-      </c>
-      <c r="H8" s="124">
-        <v>41974</v>
-      </c>
-      <c r="I8" s="127" t="str">
+      <c r="C8" s="83" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="84">
+        <v>40193</v>
+      </c>
+      <c r="E8" s="99">
+        <v>0.03</v>
+      </c>
+      <c r="F8" s="100">
+        <v>100</v>
+      </c>
+      <c r="G8" s="84">
+        <v>38367</v>
+      </c>
+      <c r="H8" s="97">
+        <v>38369</v>
+      </c>
+      <c r="I8" s="88" t="str">
         <f>_xll.qlBTP2(C8,,D8,E8,F8,G8,H8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0005069395#0007</v>
-      </c>
-      <c r="J8" s="128" t="b">
+        <v>IT0003799597#0001</v>
+      </c>
+      <c r="J8" s="123" t="b">
         <v>0</v>
       </c>
-      <c r="K8" s="56" t="str">
+      <c r="K8" s="121" t="str">
         <f>IF(AND(J8,ISNA(L8),ISNA(M8)),"Residual Missing","--")</f>
         <v>--</v>
       </c>
@@ -4785,40 +4752,43 @@
         <v>#N/A</v>
       </c>
       <c r="N8" s="23"/>
+      <c r="R8" s="18" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="9" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="19"/>
-      <c r="B9" s="129" t="str">
+      <c r="B9" s="122" t="str">
         <f>_xll.ohRangeRetrieveError(I9)</f>
         <v/>
       </c>
       <c r="C9" s="83" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D9" s="84">
-        <v>40193</v>
+        <v>40238</v>
       </c>
       <c r="E9" s="99">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="F9" s="100">
         <v>100</v>
       </c>
       <c r="G9" s="84">
-        <v>38367</v>
+        <v>39142</v>
       </c>
       <c r="H9" s="97">
-        <v>38369</v>
+        <v>39142</v>
       </c>
       <c r="I9" s="88" t="str">
         <f>_xll.qlBTP2(C9,,D9,E9,F9,G9,H9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003799597#0014</v>
-      </c>
-      <c r="J9" s="130" t="b">
+        <v>IT0004196918#0001</v>
+      </c>
+      <c r="J9" s="123" t="b">
         <v>0</v>
       </c>
       <c r="K9" s="121" t="str">
-        <f>IF(AND(J9,ISNA(L9),ISNA(M9)),"Residual Missing","--")</f>
+        <f t="shared" ref="K9:K76" si="0">IF(AND(J9,ISNA(L9),ISNA(M9)),"Residual Missing","--")</f>
         <v>--</v>
       </c>
       <c r="L9" s="48" t="e">
@@ -4830,43 +4800,40 @@
         <v>#N/A</v>
       </c>
       <c r="N9" s="23"/>
-      <c r="R9" s="18" t="s">
-        <v>380</v>
-      </c>
     </row>
     <row r="10" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
-      <c r="B10" s="129" t="str">
+      <c r="B10" s="122" t="str">
         <f>_xll.ohRangeRetrieveError(I10)</f>
         <v/>
       </c>
       <c r="C10" s="83" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D10" s="84">
-        <v>40238</v>
+        <v>40344</v>
       </c>
       <c r="E10" s="99">
-        <v>0.04</v>
+        <v>2.75E-2</v>
       </c>
       <c r="F10" s="100">
         <v>100</v>
       </c>
       <c r="G10" s="84">
-        <v>39142</v>
+        <v>38518</v>
       </c>
       <c r="H10" s="97">
-        <v>39142</v>
+        <v>38520</v>
       </c>
       <c r="I10" s="88" t="str">
         <f>_xll.qlBTP2(C10,,D10,E10,F10,G10,H10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004196918#0006</v>
-      </c>
-      <c r="J10" s="130" t="b">
+        <v>IT0003872923#0001</v>
+      </c>
+      <c r="J10" s="123" t="b">
         <v>0</v>
       </c>
       <c r="K10" s="121" t="str">
-        <f t="shared" ref="K10:K76" si="0">IF(AND(J10,ISNA(L10),ISNA(M10)),"Residual Missing","--")</f>
+        <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="L10" s="48" t="e">
@@ -4881,33 +4848,33 @@
     </row>
     <row r="11" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
-      <c r="B11" s="129" t="str">
+      <c r="B11" s="122" t="str">
         <f>_xll.ohRangeRetrieveError(I11)</f>
         <v/>
       </c>
       <c r="C11" s="83" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D11" s="84">
-        <v>40344</v>
+        <v>40391</v>
       </c>
       <c r="E11" s="99">
-        <v>2.75E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F11" s="100">
         <v>100</v>
       </c>
       <c r="G11" s="84">
-        <v>38518</v>
+        <v>39295</v>
       </c>
       <c r="H11" s="97">
-        <v>38520</v>
+        <v>39295</v>
       </c>
       <c r="I11" s="88" t="str">
         <f>_xll.qlBTP2(C11,,D11,E11,F11,G11,H11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003872923#0006</v>
-      </c>
-      <c r="J11" s="130" t="b">
+        <v>IT0004254352#0001</v>
+      </c>
+      <c r="J11" s="123" t="b">
         <v>0</v>
       </c>
       <c r="K11" s="121" t="str">
@@ -4926,126 +4893,126 @@
     </row>
     <row r="12" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
-      <c r="B12" s="129" t="str">
+      <c r="B12" s="122" t="str">
         <f>_xll.ohRangeRetrieveError(I12)</f>
         <v/>
       </c>
       <c r="C12" s="83" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="D12" s="84">
-        <v>40391</v>
+        <v>40483</v>
       </c>
       <c r="E12" s="99">
-        <v>4.4999999999999998E-2</v>
+        <v>5.5E-2</v>
       </c>
       <c r="F12" s="100">
         <v>100</v>
       </c>
       <c r="G12" s="84">
-        <v>39295</v>
+        <v>36465</v>
       </c>
       <c r="H12" s="97">
-        <v>39295</v>
+        <v>36619</v>
       </c>
       <c r="I12" s="88" t="str">
         <f>_xll.qlBTP2(C12,,D12,E12,F12,G12,H12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004254352#0006</v>
-      </c>
-      <c r="J12" s="130" t="b">
-        <v>0</v>
+        <v>IT0001448619#0001</v>
+      </c>
+      <c r="J12" s="123" t="b">
+        <v>1</v>
       </c>
       <c r="K12" s="121" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
-      <c r="L12" s="48" t="e">
+      <c r="L12" s="48" t="str">
         <f>LEFT(VLOOKUP($D12,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
-        <v>#N/A</v>
+        <v>IT0001461844</v>
       </c>
       <c r="M12" s="120" t="e">
         <f>LEFT(VLOOKUP($D12,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
       <c r="N12" s="23"/>
+      <c r="R12" s="18" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="13" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
-      <c r="B13" s="129" t="str">
+      <c r="B13" s="122" t="str">
         <f>_xll.ohRangeRetrieveError(I13)</f>
         <v/>
       </c>
       <c r="C13" s="83" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="D13" s="84">
-        <v>40483</v>
+        <v>40575</v>
       </c>
       <c r="E13" s="99">
-        <v>5.5E-2</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="F13" s="100">
         <v>100</v>
       </c>
       <c r="G13" s="84">
-        <v>36465</v>
+        <v>39479</v>
       </c>
       <c r="H13" s="97">
-        <v>36619</v>
+        <v>39510</v>
       </c>
       <c r="I13" s="88" t="str">
         <f>_xll.qlBTP2(C13,,D13,E13,F13,G13,H13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0001448619#0006</v>
-      </c>
-      <c r="J13" s="130" t="b">
-        <v>1</v>
+        <v>IT0004332521#0001</v>
+      </c>
+      <c r="J13" s="123" t="b">
+        <v>0</v>
       </c>
       <c r="K13" s="121" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
-      <c r="L13" s="48" t="str">
+      <c r="L13" s="48" t="e">
         <f>LEFT(VLOOKUP($D13,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
-        <v>IT0001461844</v>
+        <v>#N/A</v>
       </c>
       <c r="M13" s="120" t="e">
         <f>LEFT(VLOOKUP($D13,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
       <c r="N13" s="23"/>
-      <c r="R13" s="18" t="s">
-        <v>380</v>
-      </c>
     </row>
     <row r="14" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
-      <c r="B14" s="129" t="str">
+      <c r="B14" s="122" t="str">
         <f>_xll.ohRangeRetrieveError(I14)</f>
         <v/>
       </c>
       <c r="C14" s="83" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D14" s="84">
-        <v>40575</v>
+        <v>40617</v>
       </c>
       <c r="E14" s="99">
-        <v>3.7499999999999999E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="F14" s="100">
         <v>100</v>
       </c>
       <c r="G14" s="84">
-        <v>39479</v>
+        <v>38791</v>
       </c>
       <c r="H14" s="97">
-        <v>39510</v>
+        <v>38791</v>
       </c>
       <c r="I14" s="88" t="str">
         <f>_xll.qlBTP2(C14,,D14,E14,F14,G14,H14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004332521#0006</v>
-      </c>
-      <c r="J14" s="130" t="b">
+        <v>IT0004026297#0001</v>
+      </c>
+      <c r="J14" s="123" t="b">
         <v>0</v>
       </c>
       <c r="K14" s="121" t="str">
@@ -5064,34 +5031,34 @@
     </row>
     <row r="15" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
-      <c r="B15" s="129" t="str">
+      <c r="B15" s="122" t="str">
         <f>_xll.ohRangeRetrieveError(I15)</f>
         <v/>
       </c>
       <c r="C15" s="83" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="D15" s="84">
-        <v>40617</v>
+        <v>40756</v>
       </c>
       <c r="E15" s="99">
-        <v>3.5000000000000003E-2</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="F15" s="100">
         <v>100</v>
       </c>
       <c r="G15" s="84">
-        <v>38791</v>
+        <v>36923</v>
       </c>
       <c r="H15" s="97">
-        <v>38791</v>
+        <v>36951</v>
       </c>
       <c r="I15" s="88" t="str">
         <f>_xll.qlBTP2(C15,,D15,E15,F15,G15,H15,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004026297#0006</v>
-      </c>
-      <c r="J15" s="130" t="b">
-        <v>0</v>
+        <v>IT0003080402#0001</v>
+      </c>
+      <c r="J15" s="123" t="b">
+        <v>1</v>
       </c>
       <c r="K15" s="121" t="str">
         <f t="shared" si="0"/>
@@ -5101,42 +5068,42 @@
         <f>LEFT(VLOOKUP($D15,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M15" s="120" t="e">
+      <c r="M15" s="120" t="str">
         <f>LEFT(VLOOKUP($D15,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>#N/A</v>
+        <v>IT0003106389</v>
       </c>
       <c r="N15" s="23"/>
     </row>
     <row r="16" spans="1:18" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
-      <c r="B16" s="129" t="str">
+      <c r="B16" s="122" t="str">
         <f>_xll.ohRangeRetrieveError(I16)</f>
         <v/>
       </c>
       <c r="C16" s="83" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D16" s="84">
-        <v>40756</v>
+        <v>40787</v>
       </c>
       <c r="E16" s="99">
-        <v>5.2499999999999998E-2</v>
+        <v>4.2500000000000003E-2</v>
       </c>
       <c r="F16" s="100">
         <v>100</v>
       </c>
       <c r="G16" s="84">
-        <v>36923</v>
+        <v>39692</v>
       </c>
       <c r="H16" s="97">
-        <v>36951</v>
+        <v>39692</v>
       </c>
       <c r="I16" s="88" t="str">
         <f>_xll.qlBTP2(C16,,D16,E16,F16,G16,H16,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003080402#0006</v>
-      </c>
-      <c r="J16" s="130" t="b">
-        <v>1</v>
+        <v>IT0004404973#0001</v>
+      </c>
+      <c r="J16" s="123" t="b">
+        <v>0</v>
       </c>
       <c r="K16" s="121" t="str">
         <f t="shared" si="0"/>
@@ -5146,41 +5113,41 @@
         <f>LEFT(VLOOKUP($D16,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M16" s="120" t="str">
+      <c r="M16" s="120" t="e">
         <f>LEFT(VLOOKUP($D16,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>IT0003106389</v>
-      </c>
-      <c r="N16" s="23"/>
+        <v>#N/A</v>
+      </c>
+      <c r="N16" s="27"/>
     </row>
     <row r="17" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19"/>
-      <c r="B17" s="129" t="str">
+      <c r="B17" s="122" t="str">
         <f>_xll.ohRangeRetrieveError(I17)</f>
         <v/>
       </c>
       <c r="C17" s="83" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D17" s="84">
-        <v>40787</v>
+        <v>40801</v>
       </c>
       <c r="E17" s="99">
-        <v>4.2500000000000003E-2</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="F17" s="100">
         <v>100</v>
       </c>
       <c r="G17" s="84">
-        <v>39692</v>
+        <v>38975</v>
       </c>
       <c r="H17" s="97">
-        <v>39692</v>
+        <v>38978</v>
       </c>
       <c r="I17" s="88" t="str">
         <f>_xll.qlBTP2(C17,,D17,E17,F17,G17,H17,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004404973#0006</v>
-      </c>
-      <c r="J17" s="130" t="b">
+        <v>IT0004112816#0001</v>
+      </c>
+      <c r="J17" s="123" t="b">
         <v>0</v>
       </c>
       <c r="K17" s="121" t="str">
@@ -5199,34 +5166,34 @@
     </row>
     <row r="18" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="19"/>
-      <c r="B18" s="129" t="str">
+      <c r="B18" s="122" t="str">
         <f>_xll.ohRangeRetrieveError(I18)</f>
         <v/>
       </c>
       <c r="C18" s="83" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="84">
-        <v>40801</v>
-      </c>
-      <c r="E18" s="99">
-        <v>3.7499999999999999E-2</v>
-      </c>
-      <c r="F18" s="100">
-        <v>100</v>
-      </c>
-      <c r="G18" s="84">
-        <v>38975</v>
-      </c>
-      <c r="H18" s="97">
-        <v>38978</v>
+        <v>35</v>
+      </c>
+      <c r="D18" s="89">
+        <v>40940</v>
+      </c>
+      <c r="E18" s="90">
+        <v>0.05</v>
+      </c>
+      <c r="F18" s="91">
+        <v>100</v>
+      </c>
+      <c r="G18" s="89">
+        <v>37104</v>
+      </c>
+      <c r="H18" s="89">
+        <v>37196</v>
       </c>
       <c r="I18" s="88" t="str">
         <f>_xll.qlBTP2(C18,,D18,E18,F18,G18,H18,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004112816#0006</v>
-      </c>
-      <c r="J18" s="130" t="b">
-        <v>0</v>
+        <v>IT0003190912#0001</v>
+      </c>
+      <c r="J18" s="123" t="b">
+        <v>1</v>
       </c>
       <c r="K18" s="121" t="str">
         <f t="shared" si="0"/>
@@ -5236,87 +5203,88 @@
         <f>LEFT(VLOOKUP($D18,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M18" s="120" t="e">
+      <c r="M18" s="120" t="str">
         <f>LEFT(VLOOKUP($D18,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>#N/A</v>
+        <v>IT0003204903</v>
       </c>
       <c r="N18" s="27"/>
     </row>
     <row r="19" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19"/>
-      <c r="B19" s="129" t="str">
+      <c r="B19" s="122" t="str">
         <f>_xll.ohRangeRetrieveError(I19)</f>
         <v/>
       </c>
       <c r="C19" s="83" t="s">
-        <v>35</v>
+        <v>62</v>
       </c>
       <c r="D19" s="89">
-        <v>40940</v>
+        <v>40969</v>
       </c>
       <c r="E19" s="90">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="F19" s="91">
         <v>100</v>
       </c>
       <c r="G19" s="89">
-        <v>37104</v>
+        <v>39873</v>
       </c>
       <c r="H19" s="89">
-        <v>37196</v>
+        <v>39874</v>
       </c>
       <c r="I19" s="88" t="str">
         <f>_xll.qlBTP2(C19,,D19,E19,F19,G19,H19,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003190912#0006</v>
-      </c>
-      <c r="J19" s="130" t="b">
-        <v>1</v>
+        <v>IT0004467483#0001</v>
+      </c>
+      <c r="J19" s="123" t="b">
+        <f t="shared" ref="J19:J90" si="1">NOT(ISNA(VLOOKUP(LEFT($I19,12),LatestStrippable,1,FALSE)))</f>
+        <v>0</v>
       </c>
       <c r="K19" s="121" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
-      <c r="L19" s="48" t="e">
+      <c r="L19" s="96" t="e">
         <f>LEFT(VLOOKUP($D19,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M19" s="120" t="str">
+      <c r="M19" s="135" t="e">
         <f>LEFT(VLOOKUP($D19,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>IT0003204903</v>
+        <v>#N/A</v>
       </c>
       <c r="N19" s="27"/>
     </row>
     <row r="20" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="19"/>
-      <c r="B20" s="129" t="str">
+      <c r="B20" s="122" t="str">
         <f>_xll.ohRangeRetrieveError(I20)</f>
         <v/>
       </c>
       <c r="C20" s="83" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D20" s="89">
-        <v>40969</v>
+        <v>41014</v>
       </c>
       <c r="E20" s="90">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="F20" s="91">
         <v>100</v>
       </c>
       <c r="G20" s="89">
-        <v>39873</v>
+        <v>39187</v>
       </c>
       <c r="H20" s="89">
-        <v>39874</v>
+        <v>39189</v>
       </c>
       <c r="I20" s="88" t="str">
         <f>_xll.qlBTP2(C20,,D20,E20,F20,G20,H20,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004467483#0006</v>
-      </c>
-      <c r="J20" s="130" t="b">
-        <f t="shared" ref="J20:J90" si="1">NOT(ISNA(VLOOKUP(LEFT($I20,12),LatestStrippable,1,FALSE)))</f>
+        <v>IT0004220627#0001</v>
+      </c>
+      <c r="J20" s="123" t="b">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="K20" s="121" t="str">
@@ -5327,7 +5295,7 @@
         <f>LEFT(VLOOKUP($D20,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M20" s="142" t="e">
+      <c r="M20" s="135" t="e">
         <f>LEFT(VLOOKUP($D20,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
@@ -5335,33 +5303,33 @@
     </row>
     <row r="21" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="19"/>
-      <c r="B21" s="129" t="str">
+      <c r="B21" s="122" t="str">
         <f>_xll.ohRangeRetrieveError(I21)</f>
         <v/>
       </c>
       <c r="C21" s="83" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D21" s="89">
-        <v>41014</v>
+        <v>41091</v>
       </c>
       <c r="E21" s="90">
-        <v>0.04</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="F21" s="91">
         <v>100</v>
       </c>
       <c r="G21" s="89">
-        <v>39187</v>
+        <v>39995</v>
       </c>
       <c r="H21" s="89">
-        <v>39189</v>
+        <v>39995</v>
       </c>
       <c r="I21" s="88" t="str">
         <f>_xll.qlBTP2(C21,,D21,E21,F21,G21,H21,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004220627#0006</v>
-      </c>
-      <c r="J21" s="130" t="b">
+        <v>IT0004508971#0001</v>
+      </c>
+      <c r="J21" s="123" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5369,11 +5337,11 @@
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
-      <c r="L21" s="96" t="e">
+      <c r="L21" s="48" t="e">
         <f>LEFT(VLOOKUP($D21,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M21" s="142" t="e">
+      <c r="M21" s="120" t="e">
         <f>LEFT(VLOOKUP($D21,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
@@ -5381,33 +5349,33 @@
     </row>
     <row r="22" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="19"/>
-      <c r="B22" s="129" t="str">
+      <c r="B22" s="122" t="str">
         <f>_xll.ohRangeRetrieveError(I22)</f>
         <v/>
       </c>
       <c r="C22" s="83" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D22" s="89">
-        <v>41091</v>
+        <v>41197</v>
       </c>
       <c r="E22" s="90">
-        <v>2.5000000000000001E-2</v>
+        <v>4.2500000000000003E-2</v>
       </c>
       <c r="F22" s="91">
         <v>100</v>
       </c>
       <c r="G22" s="89">
-        <v>39995</v>
+        <v>39370</v>
       </c>
       <c r="H22" s="89">
-        <v>39995</v>
+        <v>39370</v>
       </c>
       <c r="I22" s="88" t="str">
         <f>_xll.qlBTP2(C22,,D22,E22,F22,G22,H22,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004508971#0006</v>
-      </c>
-      <c r="J22" s="130" t="b">
+        <v>IT0004284334#0001</v>
+      </c>
+      <c r="J22" s="123" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5427,33 +5395,33 @@
     </row>
     <row r="23" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="19"/>
-      <c r="B23" s="129" t="str">
+      <c r="B23" s="122" t="str">
         <f>_xll.ohRangeRetrieveError(I23)</f>
         <v/>
       </c>
       <c r="C23" s="83" t="s">
-        <v>65</v>
+        <v>349</v>
       </c>
       <c r="D23" s="89">
-        <v>41197</v>
+        <v>41258</v>
       </c>
       <c r="E23" s="90">
-        <v>4.2500000000000003E-2</v>
+        <v>0.02</v>
       </c>
       <c r="F23" s="91">
         <v>100</v>
       </c>
       <c r="G23" s="89">
-        <v>39370</v>
+        <v>40162</v>
       </c>
       <c r="H23" s="89">
-        <v>39370</v>
+        <v>40182</v>
       </c>
       <c r="I23" s="88" t="str">
         <f>_xll.qlBTP2(C23,,D23,E23,F23,G23,H23,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004284334#0006</v>
-      </c>
-      <c r="J23" s="130" t="b">
+        <v>IT0004564636#0001</v>
+      </c>
+      <c r="J23" s="123" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5473,35 +5441,35 @@
     </row>
     <row r="24" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="19"/>
-      <c r="B24" s="129" t="str">
+      <c r="B24" s="122" t="str">
         <f>_xll.ohRangeRetrieveError(I24)</f>
         <v/>
       </c>
       <c r="C24" s="83" t="s">
-        <v>349</v>
+        <v>36</v>
       </c>
       <c r="D24" s="89">
-        <v>41258</v>
+        <v>41306</v>
       </c>
       <c r="E24" s="90">
-        <v>0.02</v>
+        <v>4.7500000000000001E-2</v>
       </c>
       <c r="F24" s="91">
         <v>100</v>
       </c>
       <c r="G24" s="89">
-        <v>40162</v>
+        <v>37469</v>
       </c>
       <c r="H24" s="89">
-        <v>40182</v>
+        <v>37501</v>
       </c>
       <c r="I24" s="88" t="str">
         <f>_xll.qlBTP2(C24,,D24,E24,F24,G24,H24,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004564636#0006</v>
-      </c>
-      <c r="J24" s="130" t="b">
+        <v>IT0003357982#0001</v>
+      </c>
+      <c r="J24" s="123" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="121" t="str">
         <f t="shared" si="0"/>
@@ -5511,43 +5479,43 @@
         <f>LEFT(VLOOKUP($D24,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M24" s="120" t="e">
+      <c r="M24" s="120" t="str">
         <f>LEFT(VLOOKUP($D24,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>#N/A</v>
+        <v>IT0003398333</v>
       </c>
       <c r="N24" s="27"/>
     </row>
     <row r="25" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="19"/>
-      <c r="B25" s="129" t="str">
+      <c r="B25" s="122" t="str">
         <f>_xll.ohRangeRetrieveError(I25)</f>
         <v/>
       </c>
       <c r="C25" s="83" t="s">
-        <v>36</v>
+        <v>66</v>
       </c>
       <c r="D25" s="89">
-        <v>41306</v>
+        <v>41379</v>
       </c>
       <c r="E25" s="90">
-        <v>4.7500000000000001E-2</v>
+        <v>4.2500000000000003E-2</v>
       </c>
       <c r="F25" s="91">
         <v>100</v>
       </c>
       <c r="G25" s="89">
-        <v>37469</v>
+        <v>39553</v>
       </c>
       <c r="H25" s="89">
-        <v>37501</v>
+        <v>39584</v>
       </c>
       <c r="I25" s="88" t="str">
         <f>_xll.qlBTP2(C25,,D25,E25,F25,G25,H25,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003357982#0006</v>
-      </c>
-      <c r="J25" s="130" t="b">
+        <v>IT0004365554#0001</v>
+      </c>
+      <c r="J25" s="123" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K25" s="121" t="str">
         <f t="shared" si="0"/>
@@ -5557,41 +5525,41 @@
         <f>LEFT(VLOOKUP($D25,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M25" s="120" t="str">
+      <c r="M25" s="120" t="e">
         <f>LEFT(VLOOKUP($D25,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>IT0003398333</v>
+        <v>#N/A</v>
       </c>
       <c r="N25" s="27"/>
     </row>
     <row r="26" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="19"/>
-      <c r="B26" s="129" t="str">
+      <c r="B26" s="124" t="str">
         <f>_xll.ohRangeRetrieveError(I26)</f>
         <v/>
       </c>
-      <c r="C26" s="83" t="s">
-        <v>66</v>
-      </c>
-      <c r="D26" s="89">
-        <v>41379</v>
-      </c>
-      <c r="E26" s="90">
-        <v>4.2500000000000003E-2</v>
-      </c>
-      <c r="F26" s="91">
-        <v>100</v>
-      </c>
-      <c r="G26" s="89">
-        <v>39553</v>
-      </c>
-      <c r="H26" s="89">
-        <v>39584</v>
+      <c r="C26" s="112" t="s">
+        <v>352</v>
+      </c>
+      <c r="D26" s="113">
+        <v>41426</v>
+      </c>
+      <c r="E26" s="114">
+        <v>0.02</v>
+      </c>
+      <c r="F26" s="115">
+        <v>100</v>
+      </c>
+      <c r="G26" s="113">
+        <v>40330</v>
+      </c>
+      <c r="H26" s="113">
+        <v>40330</v>
       </c>
       <c r="I26" s="88" t="str">
         <f>_xll.qlBTP2(C26,,D26,E26,F26,G26,H26,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004365554#0006</v>
-      </c>
-      <c r="J26" s="130" t="b">
+        <v>IT0004612179#0001</v>
+      </c>
+      <c r="J26" s="125" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5611,35 +5579,35 @@
     </row>
     <row r="27" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="19"/>
-      <c r="B27" s="131" t="str">
+      <c r="B27" s="124" t="str">
         <f>_xll.ohRangeRetrieveError(I27)</f>
         <v/>
       </c>
       <c r="C27" s="112" t="s">
-        <v>352</v>
+        <v>37</v>
       </c>
       <c r="D27" s="113">
-        <v>41426</v>
+        <v>41487</v>
       </c>
       <c r="E27" s="114">
-        <v>0.02</v>
+        <v>4.2500000000000003E-2</v>
       </c>
       <c r="F27" s="115">
         <v>100</v>
       </c>
       <c r="G27" s="113">
-        <v>40330</v>
+        <v>37653</v>
       </c>
       <c r="H27" s="113">
-        <v>40330</v>
+        <v>37743</v>
       </c>
       <c r="I27" s="88" t="str">
         <f>_xll.qlBTP2(C27,,D27,E27,F27,G27,H27,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004612179#0006</v>
-      </c>
-      <c r="J27" s="132" t="b">
+        <v>IT0003472336#0001</v>
+      </c>
+      <c r="J27" s="125" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" s="121" t="str">
         <f t="shared" si="0"/>
@@ -5649,43 +5617,43 @@
         <f>LEFT(VLOOKUP($D27,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M27" s="120" t="e">
+      <c r="M27" s="120" t="str">
         <f>LEFT(VLOOKUP($D27,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>#N/A</v>
+        <v>IT0003474951</v>
       </c>
       <c r="N27" s="27"/>
     </row>
     <row r="28" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="19"/>
-      <c r="B28" s="131" t="str">
+      <c r="B28" s="124" t="str">
         <f>_xll.ohRangeRetrieveError(I28)</f>
         <v/>
       </c>
       <c r="C28" s="112" t="s">
-        <v>37</v>
+        <v>405</v>
       </c>
       <c r="D28" s="113">
-        <v>41487</v>
+        <v>41579</v>
       </c>
       <c r="E28" s="114">
-        <v>4.2500000000000003E-2</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="F28" s="115">
         <v>100</v>
       </c>
       <c r="G28" s="113">
-        <v>37653</v>
+        <v>40483</v>
       </c>
       <c r="H28" s="113">
-        <v>37743</v>
+        <v>40483</v>
       </c>
       <c r="I28" s="88" t="str">
         <f>_xll.qlBTP2(C28,,D28,E28,F28,G28,H28,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003472336#0006</v>
-      </c>
-      <c r="J28" s="132" t="b">
+        <v>IT0004653108#0001</v>
+      </c>
+      <c r="J28" s="125" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28" s="121" t="str">
         <f t="shared" si="0"/>
@@ -5695,41 +5663,41 @@
         <f>LEFT(VLOOKUP($D28,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M28" s="120" t="str">
+      <c r="M28" s="120" t="e">
         <f>LEFT(VLOOKUP($D28,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>IT0003474951</v>
+        <v>#N/A</v>
       </c>
       <c r="N28" s="27"/>
     </row>
     <row r="29" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="19"/>
-      <c r="B29" s="131" t="str">
+      <c r="B29" s="124" t="str">
         <f>_xll.ohRangeRetrieveError(I29)</f>
         <v/>
       </c>
       <c r="C29" s="112" t="s">
-        <v>405</v>
+        <v>67</v>
       </c>
       <c r="D29" s="113">
-        <v>41579</v>
+        <v>41623</v>
       </c>
       <c r="E29" s="114">
-        <v>2.2499999999999999E-2</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="F29" s="115">
         <v>100</v>
       </c>
       <c r="G29" s="113">
-        <v>40483</v>
+        <v>39797</v>
       </c>
       <c r="H29" s="113">
-        <v>40483</v>
+        <v>39829</v>
       </c>
       <c r="I29" s="88" t="str">
         <f>_xll.qlBTP2(C29,,D29,E29,F29,G29,H29,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004653108#0006</v>
-      </c>
-      <c r="J29" s="132" t="b">
+        <v>IT0004448863#0001</v>
+      </c>
+      <c r="J29" s="125" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5749,33 +5717,33 @@
     </row>
     <row r="30" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="19"/>
-      <c r="B30" s="131" t="str">
+      <c r="B30" s="124" t="str">
         <f>_xll.ohRangeRetrieveError(I30)</f>
         <v/>
       </c>
       <c r="C30" s="112" t="s">
-        <v>67</v>
+        <v>406</v>
       </c>
       <c r="D30" s="113">
-        <v>41623</v>
+        <v>41730</v>
       </c>
       <c r="E30" s="114">
-        <v>3.7499999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="F30" s="115">
         <v>100</v>
       </c>
       <c r="G30" s="113">
-        <v>39797</v>
+        <v>40634</v>
       </c>
       <c r="H30" s="113">
-        <v>39829</v>
-      </c>
-      <c r="I30" s="88" t="str">
+        <v>40634</v>
+      </c>
+      <c r="I30" s="116" t="str">
         <f>_xll.qlBTP2(C30,,D30,E30,F30,G30,H30,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004448863#0006</v>
-      </c>
-      <c r="J30" s="132" t="b">
+        <v>IT0004707995#0001</v>
+      </c>
+      <c r="J30" s="125" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5795,33 +5763,33 @@
     </row>
     <row r="31" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="19"/>
-      <c r="B31" s="131" t="str">
+      <c r="B31" s="124" t="str">
         <f>_xll.ohRangeRetrieveError(I31)</f>
         <v/>
       </c>
       <c r="C31" s="112" t="s">
-        <v>406</v>
+        <v>68</v>
       </c>
       <c r="D31" s="113">
-        <v>41730</v>
+        <v>41791</v>
       </c>
       <c r="E31" s="114">
-        <v>0.03</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="F31" s="115">
         <v>100</v>
       </c>
       <c r="G31" s="113">
-        <v>40634</v>
+        <v>39965</v>
       </c>
       <c r="H31" s="113">
-        <v>40634</v>
+        <v>39979</v>
       </c>
       <c r="I31" s="116" t="str">
         <f>_xll.qlBTP2(C31,,D31,E31,F31,G31,H31,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004707995#0006</v>
-      </c>
-      <c r="J31" s="132" t="b">
+        <v>IT0004505076#0001</v>
+      </c>
+      <c r="J31" s="125" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5841,33 +5809,33 @@
     </row>
     <row r="32" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="19"/>
-      <c r="B32" s="131" t="str">
+      <c r="B32" s="124" t="str">
         <f>_xll.ohRangeRetrieveError(I32)</f>
         <v/>
       </c>
       <c r="C32" s="112" t="s">
-        <v>68</v>
+        <v>420</v>
       </c>
       <c r="D32" s="113">
-        <v>41791</v>
+        <v>41821</v>
       </c>
       <c r="E32" s="114">
-        <v>3.5000000000000003E-2</v>
+        <v>4.2500000000000003E-2</v>
       </c>
       <c r="F32" s="115">
         <v>100</v>
       </c>
       <c r="G32" s="113">
-        <v>39965</v>
+        <v>40725</v>
       </c>
       <c r="H32" s="113">
-        <v>39979</v>
+        <v>40756</v>
       </c>
       <c r="I32" s="116" t="str">
         <f>_xll.qlBTP2(C32,,D32,E32,F32,G32,H32,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004505076#0006</v>
-      </c>
-      <c r="J32" s="132" t="b">
+        <v>IT0004750409#0001</v>
+      </c>
+      <c r="J32" s="125" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -5887,15 +5855,15 @@
     </row>
     <row r="33" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="19"/>
-      <c r="B33" s="131" t="str">
+      <c r="B33" s="124" t="str">
         <f>_xll.ohRangeRetrieveError(I33)</f>
         <v/>
       </c>
       <c r="C33" s="112" t="s">
-        <v>420</v>
+        <v>38</v>
       </c>
       <c r="D33" s="113">
-        <v>41821</v>
+        <v>41852</v>
       </c>
       <c r="E33" s="114">
         <v>4.2500000000000003E-2</v>
@@ -5904,18 +5872,18 @@
         <v>100</v>
       </c>
       <c r="G33" s="113">
-        <v>40725</v>
+        <v>38018</v>
       </c>
       <c r="H33" s="113">
-        <v>40756</v>
+        <v>38019</v>
       </c>
       <c r="I33" s="116" t="str">
         <f>_xll.qlBTP2(C33,,D33,E33,F33,G33,H33,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004750409#0006</v>
-      </c>
-      <c r="J33" s="132" t="b">
+        <v>IT0003618383#0001</v>
+      </c>
+      <c r="J33" s="125" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33" s="121" t="str">
         <f t="shared" si="0"/>
@@ -5925,43 +5893,43 @@
         <f>LEFT(VLOOKUP($D33,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M33" s="120" t="e">
+      <c r="M33" s="120" t="str">
         <f>LEFT(VLOOKUP($D33,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>#N/A</v>
+        <v>IT0003631238</v>
       </c>
       <c r="N33" s="27"/>
     </row>
     <row r="34" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="19"/>
-      <c r="B34" s="131" t="str">
+      <c r="B34" s="124" t="str">
         <f>_xll.ohRangeRetrieveError(I34)</f>
         <v/>
       </c>
       <c r="C34" s="112" t="s">
-        <v>38</v>
+        <v>427</v>
       </c>
       <c r="D34" s="113">
-        <v>41852</v>
+        <v>41958</v>
       </c>
       <c r="E34" s="114">
-        <v>4.2500000000000003E-2</v>
+        <v>0.06</v>
       </c>
       <c r="F34" s="115">
         <v>100</v>
       </c>
       <c r="G34" s="113">
-        <v>38018</v>
+        <v>40862</v>
       </c>
       <c r="H34" s="113">
-        <v>38019</v>
+        <v>40878</v>
       </c>
       <c r="I34" s="116" t="str">
         <f>_xll.qlBTP2(C34,,D34,E34,F34,G34,H34,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003618383#0006</v>
-      </c>
-      <c r="J34" s="132" t="b">
+        <v>IT0004780380#0001</v>
+      </c>
+      <c r="J34" s="125" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K34" s="121" t="str">
         <f t="shared" si="0"/>
@@ -5971,43 +5939,43 @@
         <f>LEFT(VLOOKUP($D34,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M34" s="120" t="str">
+      <c r="M34" s="120" t="e">
         <f>LEFT(VLOOKUP($D34,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>IT0003631238</v>
+        <v>#N/A</v>
       </c>
       <c r="N34" s="27"/>
     </row>
     <row r="35" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="19"/>
-      <c r="B35" s="131" t="str">
+      <c r="B35" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I35)</f>
         <v/>
       </c>
-      <c r="C35" s="112" t="s">
-        <v>427</v>
-      </c>
-      <c r="D35" s="113">
-        <v>41958</v>
-      </c>
-      <c r="E35" s="114">
-        <v>0.06</v>
-      </c>
-      <c r="F35" s="115">
-        <v>100</v>
-      </c>
-      <c r="G35" s="113">
-        <v>40862</v>
-      </c>
-      <c r="H35" s="113">
-        <v>40878</v>
-      </c>
-      <c r="I35" s="116" t="str">
+      <c r="C35" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="85">
+        <v>42036</v>
+      </c>
+      <c r="E35" s="86">
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="F35" s="87">
+        <v>100</v>
+      </c>
+      <c r="G35" s="85">
+        <v>38200</v>
+      </c>
+      <c r="H35" s="85">
+        <v>38231</v>
+      </c>
+      <c r="I35" s="119" t="str">
         <f>_xll.qlBTP2(C35,,D35,E35,F35,G35,H35,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004780380#0006</v>
-      </c>
-      <c r="J35" s="132" t="b">
+        <v>IT0003719918#0001</v>
+      </c>
+      <c r="J35" s="127" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K35" s="121" t="str">
         <f t="shared" si="0"/>
@@ -6017,43 +5985,43 @@
         <f>LEFT(VLOOKUP($D35,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M35" s="120" t="e">
+      <c r="M35" s="120" t="str">
         <f>LEFT(VLOOKUP($D35,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>#N/A</v>
+        <v>IT0003725261</v>
       </c>
       <c r="N35" s="27"/>
     </row>
     <row r="36" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="19"/>
-      <c r="B36" s="133" t="str">
+      <c r="B36" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I36)</f>
         <v/>
       </c>
       <c r="C36" s="40" t="s">
-        <v>39</v>
+        <v>429</v>
       </c>
       <c r="D36" s="85">
-        <v>42036</v>
+        <v>42064</v>
       </c>
       <c r="E36" s="86">
-        <v>4.2500000000000003E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="F36" s="87">
         <v>100</v>
       </c>
       <c r="G36" s="85">
-        <v>38200</v>
+        <v>40969</v>
       </c>
       <c r="H36" s="85">
-        <v>38231</v>
+        <v>40984</v>
       </c>
       <c r="I36" s="119" t="str">
         <f>_xll.qlBTP2(C36,,D36,E36,F36,G36,H36,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003719918#0006</v>
-      </c>
-      <c r="J36" s="134" t="b">
+        <v>IT0004805070#0001</v>
+      </c>
+      <c r="J36" s="127" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K36" s="121" t="str">
         <f t="shared" si="0"/>
@@ -6063,41 +6031,41 @@
         <f>LEFT(VLOOKUP($D36,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M36" s="120" t="str">
+      <c r="M36" s="120" t="e">
         <f>LEFT(VLOOKUP($D36,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>IT0003725261</v>
+        <v>#N/A</v>
       </c>
       <c r="N36" s="27"/>
     </row>
     <row r="37" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="19"/>
-      <c r="B37" s="133" t="str">
+      <c r="B37" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I37)</f>
         <v/>
       </c>
       <c r="C37" s="40" t="s">
-        <v>429</v>
+        <v>350</v>
       </c>
       <c r="D37" s="85">
-        <v>42064</v>
+        <v>42109</v>
       </c>
       <c r="E37" s="86">
-        <v>2.5000000000000001E-2</v>
+        <v>0.03</v>
       </c>
       <c r="F37" s="87">
         <v>100</v>
       </c>
       <c r="G37" s="85">
-        <v>40969</v>
+        <v>40193</v>
       </c>
       <c r="H37" s="85">
-        <v>40984</v>
+        <v>40193</v>
       </c>
       <c r="I37" s="119" t="str">
         <f>_xll.qlBTP2(C37,,D37,E37,F37,G37,H37,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004805070#0006</v>
-      </c>
-      <c r="J37" s="134" t="b">
+        <v>IT0004568272#0001</v>
+      </c>
+      <c r="J37" s="127" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6117,15 +6085,15 @@
     </row>
     <row r="38" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="19"/>
-      <c r="B38" s="133" t="str">
+      <c r="B38" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I38)</f>
         <v/>
       </c>
       <c r="C38" s="40" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="D38" s="85">
-        <v>42109</v>
+        <v>42170</v>
       </c>
       <c r="E38" s="86">
         <v>0.03</v>
@@ -6134,16 +6102,16 @@
         <v>100</v>
       </c>
       <c r="G38" s="85">
-        <v>40193</v>
+        <v>40344</v>
       </c>
       <c r="H38" s="85">
-        <v>40193</v>
+        <v>40344</v>
       </c>
       <c r="I38" s="119" t="str">
         <f>_xll.qlBTP2(C38,,D38,E38,F38,G38,H38,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004568272#0006</v>
-      </c>
-      <c r="J38" s="134" t="b">
+        <v>IT0004615917#0001</v>
+      </c>
+      <c r="J38" s="127" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6163,33 +6131,33 @@
     </row>
     <row r="39" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="19"/>
-      <c r="B39" s="133" t="str">
+      <c r="B39" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I39)</f>
         <v/>
       </c>
       <c r="C39" s="40" t="s">
-        <v>353</v>
+        <v>432</v>
       </c>
       <c r="D39" s="85">
-        <v>42170</v>
+        <v>42200</v>
       </c>
       <c r="E39" s="86">
-        <v>0.03</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="F39" s="87">
         <v>100</v>
       </c>
       <c r="G39" s="85">
-        <v>40344</v>
+        <v>41105</v>
       </c>
       <c r="H39" s="85">
-        <v>40344</v>
+        <v>41107</v>
       </c>
       <c r="I39" s="119" t="str">
         <f>_xll.qlBTP2(C39,,D39,E39,F39,G39,H39,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004615917#0006</v>
-      </c>
-      <c r="J39" s="134" t="b">
+        <v>IT0004840788#0001</v>
+      </c>
+      <c r="J39" s="127" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6209,35 +6177,35 @@
     </row>
     <row r="40" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="19"/>
-      <c r="B40" s="133" t="str">
+      <c r="B40" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I40)</f>
         <v/>
       </c>
       <c r="C40" s="40" t="s">
-        <v>432</v>
+        <v>40</v>
       </c>
       <c r="D40" s="85">
-        <v>42200</v>
+        <v>42217</v>
       </c>
       <c r="E40" s="86">
-        <v>4.4999999999999998E-2</v>
+        <v>3.7499999999999999E-2</v>
       </c>
       <c r="F40" s="87">
         <v>100</v>
       </c>
       <c r="G40" s="85">
-        <v>41105</v>
+        <v>38384</v>
       </c>
       <c r="H40" s="85">
-        <v>41107</v>
+        <v>38474</v>
       </c>
       <c r="I40" s="119" t="str">
         <f>_xll.qlBTP2(C40,,D40,E40,F40,G40,H40,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004840788#0006</v>
-      </c>
-      <c r="J40" s="134" t="b">
+        <v>IT0003844534#0001</v>
+      </c>
+      <c r="J40" s="127" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K40" s="121" t="str">
         <f t="shared" si="0"/>
@@ -6247,225 +6215,225 @@
         <f>LEFT(VLOOKUP($D40,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M40" s="120" t="e">
+      <c r="M40" s="120" t="str">
         <f>LEFT(VLOOKUP($D40,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>#N/A</v>
+        <v>IT0003850374</v>
       </c>
       <c r="N40" s="27"/>
     </row>
     <row r="41" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="19"/>
-      <c r="B41" s="133" t="str">
+      <c r="B41" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I41)</f>
         <v/>
       </c>
       <c r="C41" s="40" t="s">
-        <v>40</v>
+        <v>407</v>
       </c>
       <c r="D41" s="85">
-        <v>42217</v>
+        <v>42309</v>
       </c>
       <c r="E41" s="86">
-        <v>3.7499999999999999E-2</v>
+        <v>0.03</v>
       </c>
       <c r="F41" s="87">
         <v>100</v>
       </c>
       <c r="G41" s="85">
-        <v>38384</v>
+        <v>40483</v>
       </c>
       <c r="H41" s="85">
-        <v>38474</v>
+        <v>40498</v>
       </c>
       <c r="I41" s="119" t="str">
         <f>_xll.qlBTP2(C41,,D41,E41,F41,G41,H41,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003844534#0006</v>
-      </c>
-      <c r="J41" s="134" t="b">
+        <v>IT0004656275#0001</v>
+      </c>
+      <c r="J41" s="127" t="b">
+        <v>1</v>
+      </c>
+      <c r="K41" s="121" t="str">
+        <f t="shared" si="0"/>
+        <v>Residual Missing</v>
+      </c>
+      <c r="L41" s="48" t="e">
+        <f>LEFT(VLOOKUP($D41,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M41" s="120" t="e">
+        <f>LEFT(VLOOKUP($D41,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N41" s="27"/>
+    </row>
+    <row r="42" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="19"/>
+      <c r="B42" s="126" t="str">
+        <f>_xll.ohRangeRetrieveError(I42)</f>
+        <v/>
+      </c>
+      <c r="C42" s="40" t="s">
+        <v>433</v>
+      </c>
+      <c r="D42" s="85">
+        <v>42339</v>
+      </c>
+      <c r="E42" s="86">
+        <v>2.75E-2</v>
+      </c>
+      <c r="F42" s="87">
+        <v>100</v>
+      </c>
+      <c r="G42" s="85">
+        <v>41244</v>
+      </c>
+      <c r="H42" s="85">
+        <v>41260</v>
+      </c>
+      <c r="I42" s="119" t="str">
+        <f>_xll.qlBTP2(C42,,D42,E42,F42,G42,H42,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>IT0004880990#0001</v>
+      </c>
+      <c r="J42" s="127" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K42" s="121" t="str">
+        <f t="shared" si="0"/>
+        <v>--</v>
+      </c>
+      <c r="L42" s="48" t="e">
+        <f>LEFT(VLOOKUP($D42,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M42" s="120" t="e">
+        <f>LEFT(VLOOKUP($D42,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N42" s="27"/>
+    </row>
+    <row r="43" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="19"/>
+      <c r="B43" s="126" t="str">
+        <f>_xll.ohRangeRetrieveError(I43)</f>
+        <v/>
+      </c>
+      <c r="C43" s="40" t="s">
+        <v>408</v>
+      </c>
+      <c r="D43" s="85">
+        <v>42475</v>
+      </c>
+      <c r="E43" s="86">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="F43" s="87">
+        <v>100</v>
+      </c>
+      <c r="G43" s="85">
+        <v>40648</v>
+      </c>
+      <c r="H43" s="85">
+        <v>40651</v>
+      </c>
+      <c r="I43" s="119" t="str">
+        <f>_xll.qlBTP2(C43,,D43,E43,F43,G43,H43,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>IT0004712748#0001</v>
+      </c>
+      <c r="J43" s="127" t="b">
+        <v>1</v>
+      </c>
+      <c r="K43" s="121" t="str">
+        <f t="shared" si="0"/>
+        <v>Residual Missing</v>
+      </c>
+      <c r="L43" s="48" t="e">
+        <f>LEFT(VLOOKUP($D43,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M43" s="120" t="e">
+        <f>LEFT(VLOOKUP($D43,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N43" s="27"/>
+    </row>
+    <row r="44" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="19"/>
+      <c r="B44" s="126" t="str">
+        <f>_xll.ohRangeRetrieveError(I44)</f>
+        <v/>
+      </c>
+      <c r="C44" s="40" t="s">
+        <v>434</v>
+      </c>
+      <c r="D44" s="85">
+        <v>42505</v>
+      </c>
+      <c r="E44" s="86">
+        <v>2.2499999999999999E-2</v>
+      </c>
+      <c r="F44" s="87">
+        <v>100</v>
+      </c>
+      <c r="G44" s="85">
+        <v>41379</v>
+      </c>
+      <c r="H44" s="85">
+        <v>41379</v>
+      </c>
+      <c r="I44" s="119" t="str">
+        <f>_xll.qlBTP2(C44,,D44,E44,F44,G44,H44,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>IT0004917792#0001</v>
+      </c>
+      <c r="J44" s="127" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K44" s="121" t="str">
+        <f t="shared" si="0"/>
+        <v>--</v>
+      </c>
+      <c r="L44" s="48" t="e">
+        <f>LEFT(VLOOKUP($D44,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M44" s="120" t="e">
+        <f>LEFT(VLOOKUP($D44,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N44" s="27"/>
+    </row>
+    <row r="45" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="19"/>
+      <c r="B45" s="126" t="str">
+        <f>_xll.ohRangeRetrieveError(I45)</f>
+        <v/>
+      </c>
+      <c r="C45" s="40" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="85">
+        <v>42583</v>
+      </c>
+      <c r="E45" s="86">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="F45" s="87">
+        <v>100</v>
+      </c>
+      <c r="G45" s="85">
+        <v>38749</v>
+      </c>
+      <c r="H45" s="85">
+        <v>38777</v>
+      </c>
+      <c r="I45" s="119" t="str">
+        <f>_xll.qlBTP2(C45,,D45,E45,F45,G45,H45,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>IT0004019581#0001</v>
+      </c>
+      <c r="J45" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
-      </c>
-      <c r="K41" s="121" t="str">
-        <f t="shared" si="0"/>
-        <v>--</v>
-      </c>
-      <c r="L41" s="48" t="e">
-        <f>LEFT(VLOOKUP($D41,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M41" s="120" t="str">
-        <f>LEFT(VLOOKUP($D41,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>IT0003850374</v>
-      </c>
-      <c r="N41" s="27"/>
-    </row>
-    <row r="42" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="19"/>
-      <c r="B42" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I42)</f>
-        <v/>
-      </c>
-      <c r="C42" s="40" t="s">
-        <v>407</v>
-      </c>
-      <c r="D42" s="85">
-        <v>42309</v>
-      </c>
-      <c r="E42" s="86">
-        <v>0.03</v>
-      </c>
-      <c r="F42" s="87">
-        <v>100</v>
-      </c>
-      <c r="G42" s="85">
-        <v>40483</v>
-      </c>
-      <c r="H42" s="85">
-        <v>40498</v>
-      </c>
-      <c r="I42" s="119" t="str">
-        <f>_xll.qlBTP2(C42,,D42,E42,F42,G42,H42,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004656275#0006</v>
-      </c>
-      <c r="J42" s="134" t="b">
-        <v>1</v>
-      </c>
-      <c r="K42" s="121" t="str">
-        <f t="shared" si="0"/>
-        <v>Residual Missing</v>
-      </c>
-      <c r="L42" s="48" t="e">
-        <f>LEFT(VLOOKUP($D42,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M42" s="120" t="e">
-        <f>LEFT(VLOOKUP($D42,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N42" s="27"/>
-    </row>
-    <row r="43" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="19"/>
-      <c r="B43" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I43)</f>
-        <v/>
-      </c>
-      <c r="C43" s="40" t="s">
-        <v>433</v>
-      </c>
-      <c r="D43" s="85">
-        <v>42339</v>
-      </c>
-      <c r="E43" s="86">
-        <v>2.75E-2</v>
-      </c>
-      <c r="F43" s="87">
-        <v>100</v>
-      </c>
-      <c r="G43" s="85">
-        <v>41244</v>
-      </c>
-      <c r="H43" s="85">
-        <v>41260</v>
-      </c>
-      <c r="I43" s="119" t="str">
-        <f>_xll.qlBTP2(C43,,D43,E43,F43,G43,H43,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004880990#0006</v>
-      </c>
-      <c r="J43" s="134" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K43" s="121" t="str">
-        <f t="shared" si="0"/>
-        <v>--</v>
-      </c>
-      <c r="L43" s="48" t="e">
-        <f>LEFT(VLOOKUP($D43,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M43" s="120" t="e">
-        <f>LEFT(VLOOKUP($D43,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N43" s="27"/>
-    </row>
-    <row r="44" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="19"/>
-      <c r="B44" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I44)</f>
-        <v/>
-      </c>
-      <c r="C44" s="40" t="s">
-        <v>408</v>
-      </c>
-      <c r="D44" s="85">
-        <v>42475</v>
-      </c>
-      <c r="E44" s="86">
-        <v>3.7499999999999999E-2</v>
-      </c>
-      <c r="F44" s="87">
-        <v>100</v>
-      </c>
-      <c r="G44" s="85">
-        <v>40648</v>
-      </c>
-      <c r="H44" s="85">
-        <v>40651</v>
-      </c>
-      <c r="I44" s="119" t="str">
-        <f>_xll.qlBTP2(C44,,D44,E44,F44,G44,H44,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004712748#0006</v>
-      </c>
-      <c r="J44" s="134" t="b">
-        <v>1</v>
-      </c>
-      <c r="K44" s="121" t="str">
-        <f t="shared" si="0"/>
-        <v>Residual Missing</v>
-      </c>
-      <c r="L44" s="48" t="e">
-        <f>LEFT(VLOOKUP($D44,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M44" s="120" t="e">
-        <f>LEFT(VLOOKUP($D44,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N44" s="27"/>
-    </row>
-    <row r="45" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="19"/>
-      <c r="B45" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I45)</f>
-        <v/>
-      </c>
-      <c r="C45" s="40" t="s">
-        <v>434</v>
-      </c>
-      <c r="D45" s="85">
-        <v>42505</v>
-      </c>
-      <c r="E45" s="86">
-        <v>2.2499999999999999E-2</v>
-      </c>
-      <c r="F45" s="87">
-        <v>100</v>
-      </c>
-      <c r="G45" s="85">
-        <v>41379</v>
-      </c>
-      <c r="H45" s="85">
-        <v>41379</v>
-      </c>
-      <c r="I45" s="119" t="str">
-        <f>_xll.qlBTP2(C45,,D45,E45,F45,G45,H45,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004917792#0006</v>
-      </c>
-      <c r="J45" s="134" t="b">
-        <f t="shared" si="1"/>
-        <v>0</v>
       </c>
       <c r="K45" s="121" t="str">
         <f t="shared" si="0"/>
@@ -6475,92 +6443,89 @@
         <f>LEFT(VLOOKUP($D45,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M45" s="120" t="e">
+      <c r="M45" s="120" t="str">
         <f>LEFT(VLOOKUP($D45,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>#N/A</v>
+        <v>IT0004038318</v>
       </c>
       <c r="N45" s="27"/>
     </row>
     <row r="46" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="19"/>
-      <c r="B46" s="133" t="str">
+      <c r="B46" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I46)</f>
         <v/>
       </c>
       <c r="C46" s="40" t="s">
-        <v>30</v>
+        <v>422</v>
       </c>
       <c r="D46" s="85">
-        <v>42583</v>
+        <v>42628</v>
       </c>
       <c r="E46" s="86">
-        <v>3.7499999999999999E-2</v>
+        <v>4.7500000000000001E-2</v>
       </c>
       <c r="F46" s="87">
         <v>100</v>
       </c>
       <c r="G46" s="85">
-        <v>38749</v>
+        <v>40801</v>
       </c>
       <c r="H46" s="85">
-        <v>38777</v>
+        <v>40801</v>
       </c>
       <c r="I46" s="119" t="str">
         <f>_xll.qlBTP2(C46,,D46,E46,F46,G46,H46,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004019581#0006</v>
-      </c>
-      <c r="J46" s="134" t="b">
-        <f t="shared" si="1"/>
+        <v>IT0004761950#0001</v>
+      </c>
+      <c r="J46" s="127" t="b">
         <v>1</v>
       </c>
       <c r="K46" s="121" t="str">
         <f t="shared" si="0"/>
-        <v>--</v>
+        <v>Residual Missing</v>
       </c>
       <c r="L46" s="48" t="e">
         <f>LEFT(VLOOKUP($D46,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M46" s="120" t="str">
+      <c r="M46" s="120" t="e">
         <f>LEFT(VLOOKUP($D46,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>IT0004038318</v>
+        <v>#N/A</v>
       </c>
       <c r="N46" s="27"/>
     </row>
     <row r="47" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="19"/>
-      <c r="B47" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I47)</f>
-        <v/>
-      </c>
+      <c r="B47" s="126"/>
       <c r="C47" s="40" t="s">
-        <v>422</v>
+        <v>443</v>
       </c>
       <c r="D47" s="85">
-        <v>42628</v>
+        <v>42689</v>
       </c>
       <c r="E47" s="86">
-        <v>4.7500000000000001E-2</v>
+        <v>2.75E-2</v>
       </c>
       <c r="F47" s="87">
         <v>100</v>
       </c>
       <c r="G47" s="85">
-        <v>40801</v>
+        <v>41533</v>
       </c>
       <c r="H47" s="85">
-        <v>40801</v>
+        <v>41533</v>
       </c>
       <c r="I47" s="119" t="str">
         <f>_xll.qlBTP2(C47,,D47,E47,F47,G47,H47,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004761950#0006</v>
-      </c>
-      <c r="J47" s="134" t="b">
-        <v>1</v>
+        <v>IT0004960826#0001</v>
+      </c>
+      <c r="J47" s="127" t="b">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="K47" s="121" t="str">
-        <f t="shared" si="0"/>
-        <v>Residual Missing</v>
+        <f>IF(AND(J47,ISNA(L47),ISNA(M47)),"Residual Missing","--")</f>
+        <v>--</v>
       </c>
       <c r="L47" s="48" t="e">
         <f>LEFT(VLOOKUP($D47,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
@@ -6574,30 +6539,30 @@
     </row>
     <row r="48" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="19"/>
-      <c r="B48" s="133"/>
+      <c r="B48" s="126"/>
       <c r="C48" s="40" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="D48" s="85">
-        <v>42689</v>
+        <v>42719</v>
       </c>
       <c r="E48" s="86">
-        <v>2.75E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F48" s="87">
         <v>100</v>
       </c>
       <c r="G48" s="85">
-        <v>41533</v>
+        <v>41654</v>
       </c>
       <c r="H48" s="85">
-        <v>41533</v>
+        <v>41654</v>
       </c>
       <c r="I48" s="119" t="str">
         <f>_xll.qlBTP2(C48,,D48,E48,F48,G48,H48,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004960826#0006</v>
-      </c>
-      <c r="J48" s="134" t="b">
+        <v>IT0004987191#0001</v>
+      </c>
+      <c r="J48" s="127" t="b">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6617,104 +6582,106 @@
     </row>
     <row r="49" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="19"/>
-      <c r="B49" s="133"/>
+      <c r="B49" s="126" t="str">
+        <f>_xll.ohRangeRetrieveError(I49)</f>
+        <v/>
+      </c>
       <c r="C49" s="40" t="s">
-        <v>445</v>
+        <v>41</v>
       </c>
       <c r="D49" s="85">
-        <v>42719</v>
+        <v>42767</v>
       </c>
       <c r="E49" s="86">
-        <v>1.4999999999999999E-2</v>
+        <v>0.04</v>
       </c>
       <c r="F49" s="87">
         <v>100</v>
       </c>
       <c r="G49" s="85">
-        <v>41654</v>
+        <v>38930</v>
       </c>
       <c r="H49" s="85">
-        <v>41654</v>
+        <v>39084</v>
       </c>
       <c r="I49" s="119" t="str">
         <f>_xll.qlBTP2(C49,,D49,E49,F49,G49,H49,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004987191#0006</v>
-      </c>
-      <c r="J49" s="134" t="b">
+        <v>IT0004164775#0001</v>
+      </c>
+      <c r="J49" s="127" t="b">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K49" s="121" t="str">
-        <f>IF(AND(J49,ISNA(L49),ISNA(M49)),"Residual Missing","--")</f>
+        <f t="shared" si="0"/>
         <v>--</v>
       </c>
       <c r="L49" s="48" t="e">
         <f>LEFT(VLOOKUP($D49,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M49" s="120" t="e">
+      <c r="M49" s="120" t="str">
         <f>LEFT(VLOOKUP($D49,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>#N/A</v>
+        <v>IT0004276322</v>
       </c>
       <c r="N49" s="27"/>
     </row>
     <row r="50" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="19"/>
-      <c r="B50" s="133" t="str">
+      <c r="B50" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I50)</f>
         <v/>
       </c>
       <c r="C50" s="40" t="s">
-        <v>41</v>
+        <v>428</v>
       </c>
       <c r="D50" s="85">
-        <v>42767</v>
+        <v>42856</v>
       </c>
       <c r="E50" s="86">
-        <v>0.04</v>
+        <v>4.7500000000000001E-2</v>
       </c>
       <c r="F50" s="87">
         <v>100</v>
       </c>
       <c r="G50" s="85">
-        <v>38930</v>
+        <v>40940</v>
       </c>
       <c r="H50" s="85">
-        <v>39084</v>
+        <v>40940</v>
       </c>
       <c r="I50" s="119" t="str">
         <f>_xll.qlBTP2(C50,,D50,E50,F50,G50,H50,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004164775#0006</v>
-      </c>
-      <c r="J50" s="134" t="b">
-        <f t="shared" si="1"/>
+        <v>IT0004793474#0001</v>
+      </c>
+      <c r="J50" s="127" t="b">
         <v>1</v>
       </c>
       <c r="K50" s="121" t="str">
         <f t="shared" si="0"/>
-        <v>--</v>
+        <v>Residual Missing</v>
       </c>
       <c r="L50" s="48" t="e">
         <f>LEFT(VLOOKUP($D50,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M50" s="120" t="str">
+      <c r="M50" s="120" t="e">
         <f>LEFT(VLOOKUP($D50,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>IT0004276322</v>
+        <v>#N/A</v>
       </c>
       <c r="N50" s="27"/>
     </row>
     <row r="51" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="19"/>
-      <c r="B51" s="133" t="str">
+      <c r="B51" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I51)</f>
         <v/>
       </c>
       <c r="C51" s="40" t="s">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="D51" s="85">
-        <v>42856</v>
+        <v>42887</v>
       </c>
       <c r="E51" s="86">
         <v>4.7500000000000001E-2</v>
@@ -6723,16 +6690,16 @@
         <v>100</v>
       </c>
       <c r="G51" s="85">
-        <v>40940</v>
+        <v>41061</v>
       </c>
       <c r="H51" s="85">
-        <v>40940</v>
+        <v>41061</v>
       </c>
       <c r="I51" s="119" t="str">
         <f>_xll.qlBTP2(C51,,D51,E51,F51,G51,H51,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004793474#0006</v>
-      </c>
-      <c r="J51" s="134" t="b">
+        <v>IT0004820426#0001</v>
+      </c>
+      <c r="J51" s="127" t="b">
         <v>1</v>
       </c>
       <c r="K51" s="121" t="str">
@@ -6751,400 +6718,398 @@
     </row>
     <row r="52" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="19"/>
-      <c r="B52" s="133" t="str">
+      <c r="B52" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I52)</f>
         <v/>
       </c>
       <c r="C52" s="40" t="s">
-        <v>435</v>
+        <v>42</v>
       </c>
       <c r="D52" s="85">
-        <v>42887</v>
+        <v>42948</v>
       </c>
       <c r="E52" s="86">
-        <v>4.7500000000000001E-2</v>
+        <v>5.2499999999999998E-2</v>
       </c>
       <c r="F52" s="87">
         <v>100</v>
       </c>
       <c r="G52" s="85">
-        <v>41061</v>
+        <v>37288</v>
       </c>
       <c r="H52" s="85">
-        <v>41061</v>
+        <v>37301</v>
       </c>
       <c r="I52" s="119" t="str">
         <f>_xll.qlBTP2(C52,,D52,E52,F52,G52,H52,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004820426#0006</v>
-      </c>
-      <c r="J52" s="134" t="b">
+        <v>IT0003242747#0001</v>
+      </c>
+      <c r="J52" s="127" t="b">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K52" s="121" t="str">
         <f t="shared" si="0"/>
-        <v>Residual Missing</v>
+        <v>--</v>
       </c>
       <c r="L52" s="48" t="e">
         <f>LEFT(VLOOKUP($D52,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M52" s="120" t="e">
+      <c r="M52" s="120" t="str">
         <f>LEFT(VLOOKUP($D52,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>#N/A</v>
+        <v>IT0003246250</v>
       </c>
       <c r="N52" s="27"/>
     </row>
     <row r="53" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="19"/>
-      <c r="B53" s="133" t="str">
+      <c r="B53" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I53)</f>
         <v/>
       </c>
       <c r="C53" s="40" t="s">
-        <v>42</v>
+        <v>436</v>
       </c>
       <c r="D53" s="85">
-        <v>42948</v>
+        <v>43040</v>
       </c>
       <c r="E53" s="86">
-        <v>5.2499999999999998E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="F53" s="87">
         <v>100</v>
       </c>
       <c r="G53" s="85">
-        <v>37288</v>
+        <v>41214</v>
       </c>
       <c r="H53" s="85">
-        <v>37301</v>
+        <v>41214</v>
       </c>
       <c r="I53" s="119" t="str">
         <f>_xll.qlBTP2(C53,,D53,E53,F53,G53,H53,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003242747#0006</v>
-      </c>
-      <c r="J53" s="134" t="b">
+        <v>IT0004867070#0001</v>
+      </c>
+      <c r="J53" s="127" t="b">
+        <v>1</v>
+      </c>
+      <c r="K53" s="121" t="str">
+        <f t="shared" si="0"/>
+        <v>Residual Missing</v>
+      </c>
+      <c r="L53" s="48" t="e">
+        <f>LEFT(VLOOKUP($D53,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M53" s="120" t="e">
+        <f>LEFT(VLOOKUP($D53,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N53" s="27"/>
+    </row>
+    <row r="54" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="19"/>
+      <c r="B54" s="126" t="str">
+        <f>_xll.ohRangeRetrieveError(I54)</f>
+        <v/>
+      </c>
+      <c r="C54" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="D54" s="85">
+        <v>43132</v>
+      </c>
+      <c r="E54" s="86">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F54" s="87">
+        <v>100</v>
+      </c>
+      <c r="G54" s="85">
+        <v>39295</v>
+      </c>
+      <c r="H54" s="85">
+        <v>39328</v>
+      </c>
+      <c r="I54" s="119" t="str">
+        <f>_xll.qlBTP2(C54,,D54,E54,F54,G54,H54,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>IT0004273493#0001</v>
+      </c>
+      <c r="J54" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K53" s="121" t="str">
+      <c r="K54" s="121" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
-      <c r="L53" s="48" t="e">
-        <f>LEFT(VLOOKUP($D53,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M53" s="120" t="str">
-        <f>LEFT(VLOOKUP($D53,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>IT0003246250</v>
-      </c>
-      <c r="N53" s="27"/>
-    </row>
-    <row r="54" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="19"/>
-      <c r="B54" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I54)</f>
-        <v/>
-      </c>
-      <c r="C54" s="40" t="s">
-        <v>436</v>
-      </c>
-      <c r="D54" s="85">
-        <v>43040</v>
-      </c>
-      <c r="E54" s="86">
+      <c r="L54" s="48" t="e">
+        <f>LEFT(VLOOKUP($D54,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M54" s="120" t="str">
+        <f>LEFT(VLOOKUP($D54,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
+        <v>IT0004275811</v>
+      </c>
+      <c r="N54" s="27"/>
+    </row>
+    <row r="55" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="19"/>
+      <c r="B55" s="126" t="str">
+        <f>_xll.ohRangeRetrieveError(I55)</f>
+        <v/>
+      </c>
+      <c r="C55" s="40" t="s">
+        <v>437</v>
+      </c>
+      <c r="D55" s="85">
+        <v>43252</v>
+      </c>
+      <c r="E55" s="86">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="F54" s="87">
-        <v>100</v>
-      </c>
-      <c r="G54" s="85">
-        <v>41214</v>
-      </c>
-      <c r="H54" s="85">
-        <v>41214</v>
-      </c>
-      <c r="I54" s="119" t="str">
-        <f>_xll.qlBTP2(C54,,D54,E54,F54,G54,H54,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004867070#0006</v>
-      </c>
-      <c r="J54" s="134" t="b">
+      <c r="F55" s="87">
+        <v>100</v>
+      </c>
+      <c r="G55" s="85">
+        <v>41366</v>
+      </c>
+      <c r="H55" s="85">
+        <v>41366</v>
+      </c>
+      <c r="I55" s="119" t="str">
+        <f>_xll.qlBTP2(C55,,D55,E55,F55,G55,H55,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>IT0004907843#0001</v>
+      </c>
+      <c r="J55" s="127" t="b">
         <v>1</v>
       </c>
-      <c r="K54" s="121" t="str">
+      <c r="K55" s="121" t="str">
         <f t="shared" si="0"/>
         <v>Residual Missing</v>
       </c>
-      <c r="L54" s="48" t="e">
-        <f>LEFT(VLOOKUP($D54,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M54" s="120" t="e">
-        <f>LEFT(VLOOKUP($D54,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N54" s="27"/>
-    </row>
-    <row r="55" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="19"/>
-      <c r="B55" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I55)</f>
-        <v/>
-      </c>
-      <c r="C55" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="D55" s="85">
-        <v>43132</v>
-      </c>
-      <c r="E55" s="86">
+      <c r="L55" s="48" t="e">
+        <f>LEFT(VLOOKUP($D55,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M55" s="120" t="e">
+        <f>LEFT(VLOOKUP($D55,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N55" s="27"/>
+    </row>
+    <row r="56" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="19"/>
+      <c r="B56" s="126" t="str">
+        <f>_xll.ohRangeRetrieveError(I56)</f>
+        <v/>
+      </c>
+      <c r="C56" s="40" t="s">
+        <v>44</v>
+      </c>
+      <c r="D56" s="85">
+        <v>43313</v>
+      </c>
+      <c r="E56" s="86">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="F55" s="87">
-        <v>100</v>
-      </c>
-      <c r="G55" s="85">
-        <v>39295</v>
-      </c>
-      <c r="H55" s="85">
-        <v>39328</v>
-      </c>
-      <c r="I55" s="119" t="str">
-        <f>_xll.qlBTP2(C55,,D55,E55,F55,G55,H55,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004273493#0006</v>
-      </c>
-      <c r="J55" s="134" t="b">
+      <c r="F56" s="87">
+        <v>100</v>
+      </c>
+      <c r="G56" s="85">
+        <v>39479</v>
+      </c>
+      <c r="H56" s="85">
+        <v>39570</v>
+      </c>
+      <c r="I56" s="119" t="str">
+        <f>_xll.qlBTP2(C56,,D56,E56,F56,G56,H56,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>IT0004361041#0001</v>
+      </c>
+      <c r="J56" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="K55" s="121" t="str">
+      <c r="K56" s="121" t="str">
         <f t="shared" si="0"/>
         <v>--</v>
       </c>
-      <c r="L55" s="48" t="e">
-        <f>LEFT(VLOOKUP($D55,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M55" s="120" t="str">
-        <f>LEFT(VLOOKUP($D55,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>IT0004275811</v>
-      </c>
-      <c r="N55" s="27"/>
-    </row>
-    <row r="56" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="19"/>
-      <c r="B56" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I56)</f>
-        <v/>
-      </c>
-      <c r="C56" s="40" t="s">
-        <v>437</v>
-      </c>
-      <c r="D56" s="85">
-        <v>43252</v>
-      </c>
-      <c r="E56" s="86">
+      <c r="L56" s="48" t="e">
+        <f>LEFT(VLOOKUP($D56,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M56" s="120" t="str">
+        <f>LEFT(VLOOKUP($D56,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
+        <v>IT0004363450</v>
+      </c>
+      <c r="N56" s="27"/>
+    </row>
+    <row r="57" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="19"/>
+      <c r="B57" s="126"/>
+      <c r="C57" s="40" t="s">
+        <v>442</v>
+      </c>
+      <c r="D57" s="85">
+        <v>43435</v>
+      </c>
+      <c r="E57" s="86">
         <v>3.5000000000000003E-2</v>
       </c>
-      <c r="F56" s="87">
-        <v>100</v>
-      </c>
-      <c r="G56" s="85">
-        <v>41366</v>
-      </c>
-      <c r="H56" s="85">
-        <v>41366</v>
-      </c>
-      <c r="I56" s="119" t="str">
-        <f>_xll.qlBTP2(C56,,D56,E56,F56,G56,H56,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004907843#0006</v>
-      </c>
-      <c r="J56" s="134" t="b">
+      <c r="F57" s="87">
+        <v>100</v>
+      </c>
+      <c r="G57" s="85">
+        <v>41426</v>
+      </c>
+      <c r="H57" s="85">
+        <v>41519</v>
+      </c>
+      <c r="I57" s="119" t="str">
+        <f>_xll.qlBTP2(C57,,D57,E57,F57,G57,H57,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>IT0004957574#0001</v>
+      </c>
+      <c r="J57" s="127" t="b">
         <v>1</v>
       </c>
-      <c r="K56" s="121" t="str">
+      <c r="K57" s="121" t="str">
+        <f>IF(AND(J57,ISNA(L57),ISNA(M57)),"Residual Missing","--")</f>
+        <v>Residual Missing</v>
+      </c>
+      <c r="L57" s="48" t="e">
+        <f>LEFT(VLOOKUP($D57,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M57" s="120" t="e">
+        <f>LEFT(VLOOKUP($D57,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="N57" s="27"/>
+    </row>
+    <row r="58" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="19"/>
+      <c r="B58" s="126" t="str">
+        <f>_xll.ohRangeRetrieveError(I58)</f>
+        <v/>
+      </c>
+      <c r="C58" s="40" t="s">
+        <v>20</v>
+      </c>
+      <c r="D58" s="85">
+        <v>43497</v>
+      </c>
+      <c r="E58" s="86">
+        <v>4.2500000000000003E-2</v>
+      </c>
+      <c r="F58" s="87">
+        <v>100</v>
+      </c>
+      <c r="G58" s="85">
+        <v>37653</v>
+      </c>
+      <c r="H58" s="85">
+        <v>37797</v>
+      </c>
+      <c r="I58" s="119" t="str">
+        <f>_xll.qlBTP2(C58,,D58,E58,F58,G58,H58,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>IT0003493258#0001</v>
+      </c>
+      <c r="J58" s="127" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K58" s="121" t="str">
+        <f t="shared" si="0"/>
+        <v>--</v>
+      </c>
+      <c r="L58" s="48" t="e">
+        <f>LEFT(VLOOKUP($D58,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="M58" s="120" t="str">
+        <f>LEFT(VLOOKUP($D58,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
+        <v>IT0003513105</v>
+      </c>
+      <c r="N58" s="27"/>
+    </row>
+    <row r="59" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="19"/>
+      <c r="B59" s="126" t="str">
+        <f>_xll.ohRangeRetrieveError(I59)</f>
+        <v/>
+      </c>
+      <c r="C59" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="D59" s="85">
+        <v>43525</v>
+      </c>
+      <c r="E59" s="86">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F59" s="87">
+        <v>100</v>
+      </c>
+      <c r="G59" s="85">
+        <v>39692</v>
+      </c>
+      <c r="H59" s="85">
+        <v>39755</v>
+      </c>
+      <c r="I59" s="119" t="str">
+        <f>_xll.qlBTP2(C59,,D59,E59,F59,G59,H59,Permanent,Trigger,ObjectOverwrite)</f>
+        <v>IT0004423957#0001</v>
+      </c>
+      <c r="J59" s="127" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="K59" s="121" t="str">
         <f t="shared" si="0"/>
         <v>Residual Missing</v>
       </c>
-      <c r="L56" s="48" t="e">
-        <f>LEFT(VLOOKUP($D56,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M56" s="120" t="e">
-        <f>LEFT(VLOOKUP($D56,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N56" s="27"/>
-    </row>
-    <row r="57" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="19"/>
-      <c r="B57" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I57)</f>
-        <v/>
-      </c>
-      <c r="C57" s="40" t="s">
-        <v>44</v>
-      </c>
-      <c r="D57" s="85">
-        <v>43313</v>
-      </c>
-      <c r="E57" s="86">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="F57" s="87">
-        <v>100</v>
-      </c>
-      <c r="G57" s="85">
-        <v>39479</v>
-      </c>
-      <c r="H57" s="85">
-        <v>39570</v>
-      </c>
-      <c r="I57" s="119" t="str">
-        <f>_xll.qlBTP2(C57,,D57,E57,F57,G57,H57,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004361041#0006</v>
-      </c>
-      <c r="J57" s="134" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K57" s="121" t="str">
-        <f t="shared" si="0"/>
-        <v>--</v>
-      </c>
-      <c r="L57" s="48" t="e">
-        <f>LEFT(VLOOKUP($D57,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M57" s="120" t="str">
-        <f>LEFT(VLOOKUP($D57,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>IT0004363450</v>
-      </c>
-      <c r="N57" s="27"/>
-    </row>
-    <row r="58" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="19"/>
-      <c r="B58" s="133"/>
-      <c r="C58" s="40" t="s">
-        <v>442</v>
-      </c>
-      <c r="D58" s="85">
-        <v>43435</v>
-      </c>
-      <c r="E58" s="86">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="F58" s="87">
-        <v>100</v>
-      </c>
-      <c r="G58" s="85">
-        <v>41426</v>
-      </c>
-      <c r="H58" s="85">
-        <v>41519</v>
-      </c>
-      <c r="I58" s="119" t="str">
-        <f>_xll.qlBTP2(C58,,D58,E58,F58,G58,H58,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004957574#0006</v>
-      </c>
-      <c r="J58" s="134" t="b">
-        <v>1</v>
-      </c>
-      <c r="K58" s="121" t="str">
-        <f>IF(AND(J58,ISNA(L58),ISNA(M58)),"Residual Missing","--")</f>
-        <v>Residual Missing</v>
-      </c>
-      <c r="L58" s="48" t="e">
-        <f>LEFT(VLOOKUP($D58,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M58" s="120" t="e">
-        <f>LEFT(VLOOKUP($D58,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N58" s="27"/>
-    </row>
-    <row r="59" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="19"/>
-      <c r="B59" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I59)</f>
-        <v/>
-      </c>
-      <c r="C59" s="40" t="s">
-        <v>20</v>
-      </c>
-      <c r="D59" s="85">
-        <v>43497</v>
-      </c>
-      <c r="E59" s="86">
-        <v>4.2500000000000003E-2</v>
-      </c>
-      <c r="F59" s="87">
-        <v>100</v>
-      </c>
-      <c r="G59" s="85">
-        <v>37653</v>
-      </c>
-      <c r="H59" s="85">
-        <v>37797</v>
-      </c>
-      <c r="I59" s="119" t="str">
-        <f>_xll.qlBTP2(C59,,D59,E59,F59,G59,H59,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003493258#0006</v>
-      </c>
-      <c r="J59" s="134" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="K59" s="121" t="str">
-        <f t="shared" si="0"/>
-        <v>--</v>
-      </c>
       <c r="L59" s="48" t="e">
         <f>LEFT(VLOOKUP($D59,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
-      <c r="M59" s="120" t="str">
+      <c r="M59" s="120" t="e">
         <f>LEFT(VLOOKUP($D59,'BTP Strip Feb-Aug'!$H$8:$M$27,6,FALSE),12)</f>
-        <v>IT0003513105</v>
+        <v>#N/A</v>
       </c>
       <c r="N59" s="27"/>
     </row>
     <row r="60" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="19"/>
-      <c r="B60" s="133" t="str">
-        <f>_xll.ohRangeRetrieveError(I60)</f>
-        <v/>
-      </c>
+      <c r="B60" s="126"/>
       <c r="C60" s="40" t="s">
-        <v>51</v>
+        <v>446</v>
       </c>
       <c r="D60" s="85">
-        <v>43525</v>
+        <v>43586</v>
       </c>
       <c r="E60" s="86">
-        <v>4.4999999999999998E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="F60" s="87">
         <v>100</v>
       </c>
       <c r="G60" s="85">
-        <v>39692</v>
+        <v>41673</v>
       </c>
       <c r="H60" s="85">
-        <v>39755</v>
+        <v>41673</v>
       </c>
       <c r="I60" s="119" t="str">
         <f>_xll.qlBTP2(C60,,D60,E60,F60,G60,H60,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004423957#0006</v>
-      </c>
-      <c r="J60" s="134" t="b">
+        <v>IT0004992308#0001</v>
+      </c>
+      <c r="J60" s="127" t="b">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K60" s="121" t="str">
-        <f t="shared" si="0"/>
-        <v>Residual Missing</v>
+        <f>IF(AND(J60,ISNA(L60),ISNA(M60)),"Residual Missing","--")</f>
+        <v>--</v>
       </c>
       <c r="L60" s="48" t="e">
         <f>LEFT(VLOOKUP($D60,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
@@ -7158,31 +7123,30 @@
     </row>
     <row r="61" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="19"/>
-      <c r="B61" s="133"/>
+      <c r="B61" s="126"/>
       <c r="C61" s="40" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="D61" s="85">
-        <v>43586</v>
+        <v>43678</v>
       </c>
       <c r="E61" s="86">
-        <v>2.5000000000000001E-2</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F61" s="87">
         <v>100</v>
       </c>
       <c r="G61" s="85">
-        <v>41673</v>
+        <v>41821</v>
       </c>
       <c r="H61" s="85">
-        <v>41673</v>
+        <v>41821</v>
       </c>
       <c r="I61" s="119" t="str">
         <f>_xll.qlBTP2(C61,,D61,E61,F61,G61,H61,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004992308#0006</v>
-      </c>
-      <c r="J61" s="134" t="b">
-        <f t="shared" si="1"/>
+        <v>IT0005030504#0001</v>
+      </c>
+      <c r="J61" s="127" t="b">
         <v>0</v>
       </c>
       <c r="K61" s="121" t="str">
@@ -7201,35 +7165,39 @@
     </row>
     <row r="62" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="19"/>
-      <c r="B62" s="133"/>
+      <c r="B62" s="126" t="str">
+        <f>_xll.ohRangeRetrieveError(I62)</f>
+        <v/>
+      </c>
       <c r="C62" s="40" t="s">
-        <v>448</v>
+        <v>52</v>
       </c>
       <c r="D62" s="85">
-        <v>43678</v>
+        <v>43709</v>
       </c>
       <c r="E62" s="86">
-        <v>1.4999999999999999E-2</v>
+        <v>4.2500000000000003E-2</v>
       </c>
       <c r="F62" s="87">
         <v>100</v>
       </c>
       <c r="G62" s="85">
-        <v>41821</v>
+        <v>39873</v>
       </c>
       <c r="H62" s="85">
-        <v>41821</v>
+        <v>39937</v>
       </c>
       <c r="I62" s="119" t="str">
         <f>_xll.qlBTP2(C62,,D62,E62,F62,G62,H62,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0005030504#0006</v>
-      </c>
-      <c r="J62" s="134" t="b">
-        <v>0</v>
+        <v>IT0004489610#0001</v>
+      </c>
+      <c r="J62" s="127" t="b">
+        <f t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="K62" s="121" t="str">
-        <f>IF(AND(J62,ISNA(L62),ISNA(M62)),"Residual Missing","--")</f>
-        <v>--</v>
+        <f t="shared" si="0"/>
+        <v>Residual Missing</v>
       </c>
       <c r="L62" s="48" t="e">
         <f>LEFT(VLOOKUP($D62,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
@@ -7243,39 +7211,38 @@
     </row>
     <row r="63" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="19"/>
-      <c r="B63" s="133" t="str">
+      <c r="B63" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I63)</f>
         <v/>
       </c>
       <c r="C63" s="40" t="s">
-        <v>52</v>
+        <v>453</v>
       </c>
       <c r="D63" s="85">
-        <v>43709</v>
+        <v>43800</v>
       </c>
       <c r="E63" s="86">
-        <v>4.2500000000000003E-2</v>
+        <v>1.0500000000000001E-2</v>
       </c>
       <c r="F63" s="87">
         <v>100</v>
       </c>
       <c r="G63" s="85">
-        <v>39873</v>
+        <v>41974</v>
       </c>
       <c r="H63" s="85">
-        <v>39937</v>
+        <v>41974</v>
       </c>
       <c r="I63" s="119" t="str">
         <f>_xll.qlBTP2(C63,,D63,E63,F63,G63,H63,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004489610#0006</v>
-      </c>
-      <c r="J63" s="134" t="b">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <v>IT0005069395#0002</v>
+      </c>
+      <c r="J63" s="127" t="b">
+        <v>0</v>
       </c>
       <c r="K63" s="121" t="str">
-        <f t="shared" si="0"/>
-        <v>Residual Missing</v>
+        <f t="shared" ref="K63" si="2">IF(AND(J63,ISNA(L63),ISNA(M63)),"Residual Missing","--")</f>
+        <v>--</v>
       </c>
       <c r="L63" s="48" t="e">
         <f>LEFT(VLOOKUP($D63,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
@@ -7289,7 +7256,7 @@
     </row>
     <row r="64" spans="1:14" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="19"/>
-      <c r="B64" s="133" t="str">
+      <c r="B64" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I64)</f>
         <v/>
       </c>
@@ -7313,9 +7280,9 @@
       </c>
       <c r="I64" s="119" t="str">
         <f>_xll.qlBTP2(C64,,D64,E64,F64,G64,H64,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003644769#0006</v>
-      </c>
-      <c r="J64" s="134" t="b">
+        <v>IT0003644769#0001</v>
+      </c>
+      <c r="J64" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -7335,7 +7302,7 @@
     </row>
     <row r="65" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="19"/>
-      <c r="B65" s="133" t="str">
+      <c r="B65" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I65)</f>
         <v/>
       </c>
@@ -7359,9 +7326,9 @@
       </c>
       <c r="I65" s="119" t="str">
         <f>_xll.qlBTP2(C65,,D65,E65,F65,G65,H65,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004536949#0006</v>
-      </c>
-      <c r="J65" s="134" t="b">
+        <v>IT0004536949#0001</v>
+      </c>
+      <c r="J65" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -7381,7 +7348,7 @@
     </row>
     <row r="66" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="19"/>
-      <c r="B66" s="133" t="str">
+      <c r="B66" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I66)</f>
         <v/>
       </c>
@@ -7405,9 +7372,9 @@
       </c>
       <c r="I66" s="119" t="str">
         <f>_xll.qlBTP2(C66,,D66,E66,F66,G66,H66,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004594930#0006</v>
-      </c>
-      <c r="J66" s="134" t="b">
+        <v>IT0004594930#0001</v>
+      </c>
+      <c r="J66" s="127" t="b">
         <v>1</v>
       </c>
       <c r="K66" s="121" t="str">
@@ -7426,7 +7393,7 @@
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A67" s="19"/>
-      <c r="B67" s="133" t="str">
+      <c r="B67" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I67)</f>
         <v/>
       </c>
@@ -7450,9 +7417,9 @@
       </c>
       <c r="I67" s="119" t="str">
         <f>_xll.qlBTP2(C67,,D67,E67,F67,G67,H67,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004634132#0006</v>
-      </c>
-      <c r="J67" s="134" t="b">
+        <v>IT0004634132#0001</v>
+      </c>
+      <c r="J67" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -7473,7 +7440,7 @@
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A68" s="19"/>
-      <c r="B68" s="133"/>
+      <c r="B68" s="126"/>
       <c r="C68" s="40" t="s">
         <v>444</v>
       </c>
@@ -7494,9 +7461,9 @@
       </c>
       <c r="I68" s="119" t="str">
         <f>_xll.qlBTP2(C68,,D68,E68,F68,G68,H68,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004966401#0006</v>
-      </c>
-      <c r="J68" s="134" t="b">
+        <v>IT0004966401#0001</v>
+      </c>
+      <c r="J68" s="127" t="b">
         <v>1</v>
       </c>
       <c r="K68" s="121" t="str">
@@ -7516,7 +7483,7 @@
     </row>
     <row r="69" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A69" s="19"/>
-      <c r="B69" s="133" t="str">
+      <c r="B69" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I69)</f>
         <v/>
       </c>
@@ -7540,9 +7507,9 @@
       </c>
       <c r="I69" s="119" t="str">
         <f>_xll.qlBTP2(C69,,D69,E69,F69,G69,H69,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004009673#0006</v>
-      </c>
-      <c r="J69" s="134" t="b">
+        <v>IT0004009673#0001</v>
+      </c>
+      <c r="J69" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -7563,7 +7530,7 @@
     </row>
     <row r="70" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A70" s="19"/>
-      <c r="B70" s="133" t="str">
+      <c r="B70" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I70)</f>
         <v/>
       </c>
@@ -7587,9 +7554,9 @@
       </c>
       <c r="I70" s="119" t="str">
         <f>_xll.qlBTP2(C70,,D70,E70,F70,G70,H70,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004695075#0006</v>
-      </c>
-      <c r="J70" s="134" t="b">
+        <v>IT0004695075#0001</v>
+      </c>
+      <c r="J70" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -7610,7 +7577,7 @@
     </row>
     <row r="71" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A71" s="19"/>
-      <c r="B71" s="133"/>
+      <c r="B71" s="126"/>
       <c r="C71" s="40" t="s">
         <v>449</v>
       </c>
@@ -7631,9 +7598,9 @@
       </c>
       <c r="I71" s="119" t="str">
         <f>_xll.qlBTP2(C71,,D71,E71,F71,G71,H71,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0005028003#0006</v>
-      </c>
-      <c r="J71" s="134" t="b">
+        <v>IT0005028003#0001</v>
+      </c>
+      <c r="J71" s="127" t="b">
         <v>0</v>
       </c>
       <c r="K71" s="121" t="str">
@@ -7653,7 +7620,7 @@
     </row>
     <row r="72" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A72" s="19"/>
-      <c r="B72" s="133" t="str">
+      <c r="B72" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I72)</f>
         <v/>
       </c>
@@ -7677,9 +7644,9 @@
       </c>
       <c r="I72" s="119" t="str">
         <f>_xll.qlBTP2(C72,,D72,E72,F72,G72,H72,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004759673#0006</v>
-      </c>
-      <c r="J72" s="134" t="b">
+        <v>IT0004759673#0001</v>
+      </c>
+      <c r="J72" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -7700,7 +7667,7 @@
     </row>
     <row r="73" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A73" s="19"/>
-      <c r="B73" s="133" t="str">
+      <c r="B73" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I73)</f>
         <v/>
       </c>
@@ -7724,9 +7691,9 @@
       </c>
       <c r="I73" s="119" t="str">
         <f>_xll.qlBTP2(C73,,D73,E73,F73,G73,H73,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004801541#0006</v>
-      </c>
-      <c r="J73" s="134" t="b">
+        <v>IT0004801541#0001</v>
+      </c>
+      <c r="J73" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -7747,7 +7714,7 @@
     </row>
     <row r="74" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A74" s="19"/>
-      <c r="B74" s="133" t="str">
+      <c r="B74" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I74)</f>
         <v/>
       </c>
@@ -7771,9 +7738,9 @@
       </c>
       <c r="I74" s="119" t="str">
         <f>_xll.qlBTP2(C74,,D74,E74,F74,G74,H74,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004848831#0006</v>
-      </c>
-      <c r="J74" s="134" t="b">
+        <v>IT0004848831#0001</v>
+      </c>
+      <c r="J74" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -7794,7 +7761,7 @@
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A75" s="19"/>
-      <c r="B75" s="133" t="str">
+      <c r="B75" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I75)</f>
         <v/>
       </c>
@@ -7818,9 +7785,9 @@
       </c>
       <c r="I75" s="119" t="str">
         <f>_xll.qlBTP2(C75,,D75,E75,F75,G75,H75,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004898034#0006</v>
-      </c>
-      <c r="J75" s="134" t="b">
+        <v>IT0004898034#0001</v>
+      </c>
+      <c r="J75" s="127" t="b">
         <v>1</v>
       </c>
       <c r="K75" s="121" t="str">
@@ -7840,7 +7807,7 @@
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A76" s="19"/>
-      <c r="B76" s="133" t="str">
+      <c r="B76" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I76)</f>
         <v/>
       </c>
@@ -7864,9 +7831,9 @@
       </c>
       <c r="I76" s="119" t="str">
         <f>_xll.qlBTP2(C76,,D76,E76,F76,G76,H76,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004356843#0006</v>
-      </c>
-      <c r="J76" s="134" t="b">
+        <v>IT0004356843#0001</v>
+      </c>
+      <c r="J76" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -7887,7 +7854,7 @@
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A77" s="19"/>
-      <c r="B77" s="133" t="str">
+      <c r="B77" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I77)</f>
         <v/>
       </c>
@@ -7911,14 +7878,14 @@
       </c>
       <c r="I77" s="119" t="str">
         <f>_xll.qlBTP2(C77,,D77,E77,F77,G77,H77,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0000366655#0006</v>
-      </c>
-      <c r="J77" s="134" t="b">
+        <v>IT0000366655#0001</v>
+      </c>
+      <c r="J77" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K77" s="121" t="str">
-        <f t="shared" ref="K77:K94" si="2">IF(AND(J77,ISNA(L77),ISNA(M77)),"Residual Missing","--")</f>
+        <f t="shared" ref="K77:K94" si="3">IF(AND(J77,ISNA(L77),ISNA(M77)),"Residual Missing","--")</f>
         <v>--</v>
       </c>
       <c r="L77" s="48" t="str">
@@ -7934,7 +7901,7 @@
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A78" s="19"/>
-      <c r="B78" s="133"/>
+      <c r="B78" s="126"/>
       <c r="C78" s="40" t="s">
         <v>441</v>
       </c>
@@ -7955,9 +7922,9 @@
       </c>
       <c r="I78" s="119" t="str">
         <f>_xll.qlBTP2(C78,,D78,E78,F78,G78,H78,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004953417#0006</v>
-      </c>
-      <c r="J78" s="134" t="b">
+        <v>IT0004953417#0001</v>
+      </c>
+      <c r="J78" s="127" t="b">
         <v>1</v>
       </c>
       <c r="K78" s="121" t="str">
@@ -7977,7 +7944,7 @@
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A79" s="19"/>
-      <c r="B79" s="133"/>
+      <c r="B79" s="126"/>
       <c r="C79" s="40" t="s">
         <v>447</v>
       </c>
@@ -7998,9 +7965,9 @@
       </c>
       <c r="I79" s="119" t="str">
         <f>_xll.qlBTP2(C79,,D79,E79,F79,G79,H79,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0005001547#0006</v>
-      </c>
-      <c r="J79" s="134" t="b">
+        <v>IT0005001547#0001</v>
+      </c>
+      <c r="J79" s="127" t="b">
         <v>1</v>
       </c>
       <c r="K79" s="121" t="str">
@@ -8020,7 +7987,7 @@
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A80" s="19"/>
-      <c r="B80" s="133"/>
+      <c r="B80" s="126"/>
       <c r="C80" s="40" t="s">
         <v>451</v>
       </c>
@@ -8041,9 +8008,9 @@
       </c>
       <c r="I80" s="119" t="str">
         <f>_xll.qlBTP2(C80,,D80,E80,F80,G80,H80,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0005045270#0006</v>
-      </c>
-      <c r="J80" s="134" t="b">
+        <v>IT0005045270#0001</v>
+      </c>
+      <c r="J80" s="127" t="b">
         <v>1</v>
       </c>
       <c r="K80" s="121" t="str">
@@ -8063,7 +8030,7 @@
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A81" s="19"/>
-      <c r="B81" s="133" t="str">
+      <c r="B81" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I81)</f>
         <v/>
       </c>
@@ -8087,13 +8054,13 @@
       </c>
       <c r="I81" s="119" t="str">
         <f>_xll.qlBTP2(C81,,D81,E81,F81,G81,H81,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004513641#0006</v>
-      </c>
-      <c r="J81" s="134" t="b">
+        <v>IT0004513641#0001</v>
+      </c>
+      <c r="J81" s="127" t="b">
         <v>1</v>
       </c>
       <c r="K81" s="121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Residual Missing</v>
       </c>
       <c r="L81" s="48" t="e">
@@ -8109,7 +8076,7 @@
     </row>
     <row r="82" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A82" s="19"/>
-      <c r="B82" s="133" t="str">
+      <c r="B82" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I82)</f>
         <v/>
       </c>
@@ -8133,14 +8100,14 @@
       </c>
       <c r="I82" s="119" t="str">
         <f>_xll.qlBTP2(C82,,D82,E82,F82,G82,H82,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004644735#0006</v>
-      </c>
-      <c r="J82" s="134" t="b">
+        <v>IT0004644735#0001</v>
+      </c>
+      <c r="J82" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K82" s="121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Residual Missing</v>
       </c>
       <c r="L82" s="48" t="e">
@@ -8156,7 +8123,7 @@
     </row>
     <row r="83" spans="1:15" s="18" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A83" s="19"/>
-      <c r="B83" s="133" t="str">
+      <c r="B83" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I83)</f>
         <v/>
       </c>
@@ -8180,14 +8147,14 @@
       </c>
       <c r="I83" s="119" t="str">
         <f>_xll.qlBTP2(C83,,D83,E83,F83,G83,H83,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0001086567#0006</v>
-      </c>
-      <c r="J83" s="134" t="b">
+        <v>IT0001086567#0001</v>
+      </c>
+      <c r="J83" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K83" s="121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>--</v>
       </c>
       <c r="L83" s="48" t="str">
@@ -8202,7 +8169,7 @@
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A84" s="19"/>
-      <c r="B84" s="133" t="str">
+      <c r="B84" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I84)</f>
         <v/>
       </c>
@@ -8226,14 +8193,14 @@
       </c>
       <c r="I84" s="119" t="str">
         <f>_xll.qlBTP2(C84,,D84,E84,F84,G84,H84,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0001174611#0006</v>
-      </c>
-      <c r="J84" s="134" t="b">
+        <v>IT0001174611#0001</v>
+      </c>
+      <c r="J84" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K84" s="121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>--</v>
       </c>
       <c r="L84" s="48" t="str">
@@ -8248,7 +8215,7 @@
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A85" s="19"/>
-      <c r="B85" s="133" t="str">
+      <c r="B85" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I85)</f>
         <v/>
       </c>
@@ -8272,13 +8239,13 @@
       </c>
       <c r="I85" s="119" t="str">
         <f>_xll.qlBTP2(C85,,D85,E85,F85,G85,H85,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004889033#0006</v>
-      </c>
-      <c r="J85" s="134" t="b">
+        <v>IT0004889033#0001</v>
+      </c>
+      <c r="J85" s="127" t="b">
         <v>1</v>
       </c>
       <c r="K85" s="121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Residual Missing</v>
       </c>
       <c r="L85" s="48" t="e">
@@ -8293,7 +8260,7 @@
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A86" s="19"/>
-      <c r="B86" s="133" t="str">
+      <c r="B86" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I86)</f>
         <v/>
       </c>
@@ -8317,14 +8284,14 @@
       </c>
       <c r="I86" s="119" t="str">
         <f>_xll.qlBTP2(C86,,D86,E86,F86,G86,H86,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0001278511#0006</v>
-      </c>
-      <c r="J86" s="134" t="b">
+        <v>IT0001278511#0001</v>
+      </c>
+      <c r="J86" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K86" s="121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>--</v>
       </c>
       <c r="L86" s="48" t="str">
@@ -8339,7 +8306,7 @@
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A87" s="19"/>
-      <c r="B87" s="133"/>
+      <c r="B87" s="126"/>
       <c r="C87" s="40" t="s">
         <v>450</v>
       </c>
@@ -8360,9 +8327,9 @@
       </c>
       <c r="I87" s="119" t="str">
         <f>_xll.qlBTP2(C87,,D87,E87,F87,G87,H87,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0005024234#0006</v>
-      </c>
-      <c r="J87" s="134" t="b">
+        <v>IT0005024234#0001</v>
+      </c>
+      <c r="J87" s="127" t="b">
         <v>0</v>
       </c>
       <c r="K87" s="121" t="str">
@@ -8381,7 +8348,7 @@
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A88" s="19"/>
-      <c r="B88" s="133" t="str">
+      <c r="B88" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I88)</f>
         <v/>
       </c>
@@ -8405,14 +8372,14 @@
       </c>
       <c r="I88" s="119" t="str">
         <f>_xll.qlBTP2(C88,,D88,E88,F88,G88,H88,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0001444378#0006</v>
-      </c>
-      <c r="J88" s="134" t="b">
+        <v>IT0001444378#0001</v>
+      </c>
+      <c r="J88" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K88" s="121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>--</v>
       </c>
       <c r="L88" s="48" t="str">
@@ -8427,7 +8394,7 @@
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A89" s="19"/>
-      <c r="B89" s="133" t="str">
+      <c r="B89" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I89)</f>
         <v/>
       </c>
@@ -8451,14 +8418,14 @@
       </c>
       <c r="I89" s="119" t="str">
         <f>_xll.qlBTP2(C89,,D89,E89,F89,G89,H89,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003256820#0006</v>
-      </c>
-      <c r="J89" s="134" t="b">
+        <v>IT0003256820#0001</v>
+      </c>
+      <c r="J89" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K89" s="121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>--</v>
       </c>
       <c r="L89" s="48" t="e">
@@ -8473,7 +8440,7 @@
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A90" s="19"/>
-      <c r="B90" s="133" t="str">
+      <c r="B90" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I90)</f>
         <v/>
       </c>
@@ -8497,14 +8464,14 @@
       </c>
       <c r="I90" s="119" t="str">
         <f>_xll.qlBTP2(C90,,D90,E90,F90,G90,H90,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003535157#0006</v>
-      </c>
-      <c r="J90" s="134" t="b">
+        <v>IT0003535157#0001</v>
+      </c>
+      <c r="J90" s="127" t="b">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="K90" s="121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>--</v>
       </c>
       <c r="L90" s="48" t="e">
@@ -8519,7 +8486,7 @@
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A91" s="19"/>
-      <c r="B91" s="133" t="str">
+      <c r="B91" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I91)</f>
         <v/>
       </c>
@@ -8543,14 +8510,14 @@
       </c>
       <c r="I91" s="119" t="str">
         <f>_xll.qlBTP2(C91,,D91,E91,F91,G91,H91,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0003934657#0006</v>
-      </c>
-      <c r="J91" s="134" t="b">
+        <v>IT0003934657#0001</v>
+      </c>
+      <c r="J91" s="127" t="b">
         <f>NOT(ISNA(VLOOKUP(LEFT($I91,12),LatestStrippable,1,FALSE)))</f>
         <v>1</v>
       </c>
       <c r="K91" s="121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>--</v>
       </c>
       <c r="L91" s="48" t="e">
@@ -8565,7 +8532,7 @@
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A92" s="19"/>
-      <c r="B92" s="133" t="str">
+      <c r="B92" s="126" t="str">
         <f>_xll.ohRangeRetrieveError(I92)</f>
         <v/>
       </c>
@@ -8589,14 +8556,14 @@
       </c>
       <c r="I92" s="119" t="str">
         <f>_xll.qlBTP2(C92,,D92,E92,F92,G92,H92,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004286966#0006</v>
-      </c>
-      <c r="J92" s="134" t="b">
+        <v>IT0004286966#0001</v>
+      </c>
+      <c r="J92" s="127" t="b">
         <f>NOT(ISNA(VLOOKUP(LEFT($I92,12),LatestStrippable,1,FALSE)))</f>
         <v>1</v>
       </c>
       <c r="K92" s="121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>--</v>
       </c>
       <c r="L92" s="48" t="e">
@@ -8611,7 +8578,7 @@
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A93" s="19"/>
-      <c r="B93" s="133"/>
+      <c r="B93" s="126"/>
       <c r="C93" s="40" t="s">
         <v>71</v>
       </c>
@@ -8632,9 +8599,9 @@
       </c>
       <c r="I93" s="119" t="str">
         <f>_xll.qlBTP2(C93,,D93,E93,F93,G93,H93,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004532559#0006</v>
-      </c>
-      <c r="J93" s="134" t="b">
+        <v>IT0004532559#0001</v>
+      </c>
+      <c r="J93" s="127" t="b">
         <f>NOT(ISNA(VLOOKUP(LEFT($I93,12),LatestStrippable,1,FALSE)))</f>
         <v>1</v>
       </c>
@@ -8654,40 +8621,40 @@
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A94" s="19"/>
-      <c r="B94" s="135" t="str">
+      <c r="B94" s="128" t="str">
         <f>_xll.ohRangeRetrieveError(I94)</f>
         <v/>
       </c>
-      <c r="C94" s="136" t="s">
+      <c r="C94" s="129" t="s">
         <v>440</v>
       </c>
-      <c r="D94" s="137">
+      <c r="D94" s="130">
         <v>52841</v>
       </c>
-      <c r="E94" s="138">
+      <c r="E94" s="131">
         <v>4.7500000000000001E-2</v>
       </c>
-      <c r="F94" s="139">
-        <v>100</v>
-      </c>
-      <c r="G94" s="137">
+      <c r="F94" s="132">
+        <v>100</v>
+      </c>
+      <c r="G94" s="130">
         <v>41334</v>
       </c>
-      <c r="H94" s="137">
+      <c r="H94" s="130">
         <v>41416</v>
       </c>
-      <c r="I94" s="140" t="str">
+      <c r="I94" s="133" t="str">
         <f>_xll.qlBTP2(C94,,D94,E94,F94,G94,H94,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>IT0004923998#0006</v>
-      </c>
-      <c r="J94" s="141" t="b">
+        <v>IT0004923998#0001</v>
+      </c>
+      <c r="J94" s="134" t="b">
         <v>1</v>
       </c>
       <c r="K94" s="121" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Residual Missing</v>
       </c>
-      <c r="L94" s="143" t="e">
+      <c r="L94" s="136" t="e">
         <f>LEFT(VLOOKUP($D94,'BTP Strip May-Nov'!$H$8:$M$13,6,FALSE),12)</f>
         <v>#N/A</v>
       </c>
@@ -8723,8 +8690,8 @@
       <c r="G96" s="22"/>
       <c r="H96" s="22"/>
       <c r="I96" s="22" t="str">
-        <f>_xll.ohGroup(J96,_xll.ohFilter(I9:I94,J9:J94),Permanent,,ObjectOverwrite)</f>
-        <v>StrippableBTPs#0008</v>
+        <f>_xll.ohGroup(J96,_xll.ohFilter(I8:I94,J8:J94),Permanent,,ObjectOverwrite)</f>
+        <v>StrippableBTPs#0005</v>
       </c>
       <c r="J96" s="22" t="s">
         <v>357</v>
@@ -8744,8 +8711,8 @@
       <c r="G97" s="45"/>
       <c r="H97" s="45"/>
       <c r="I97" s="45" t="str">
-        <f>_xll.ohGroup(J97,I9:I94,Permanent,,ObjectOverwrite)</f>
-        <v>BTPs#0008</v>
+        <f>_xll.ohGroup(J97,I8:I94,Permanent,,ObjectOverwrite)</f>
+        <v>BTPs#0003</v>
       </c>
       <c r="J97" s="45" t="s">
         <v>356</v>
@@ -8758,7 +8725,7 @@
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R8:R9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R8">
       <formula1>"Actual/Actual (ISDA),Actual/360,30/360 (Bond Basis),30E/360 (Eurobond Basis),Actual/365 (Fixed),Actual/Actual (ISMA),Actual/Actual (AFB),1/1,30/360 (Italian),Simple"</formula1>
     </dataValidation>
   </dataValidations>
@@ -8804,7 +8771,7 @@
         <v>452</v>
       </c>
       <c r="B2" s="101" t="e">
-        <f>VLOOKUP(A2,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A2,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8813,7 +8780,7 @@
         <v>452</v>
       </c>
       <c r="B3" s="101" t="e">
-        <f>VLOOKUP(A3,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A3,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8822,7 +8789,7 @@
         <v>452</v>
       </c>
       <c r="B4" s="101" t="e">
-        <f>VLOOKUP(A4,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A4,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8831,7 +8798,7 @@
         <v>452</v>
       </c>
       <c r="B5" s="101" t="e">
-        <f>VLOOKUP(A5,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A5,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8840,7 +8807,7 @@
         <v>452</v>
       </c>
       <c r="B6" s="101" t="e">
-        <f>VLOOKUP(A6,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A6,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8849,7 +8816,7 @@
         <v>452</v>
       </c>
       <c r="B7" s="101" t="e">
-        <f>VLOOKUP(A7,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A7,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8858,7 +8825,7 @@
         <v>452</v>
       </c>
       <c r="B8" s="101" t="e">
-        <f>VLOOKUP(A8,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A8,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8867,7 +8834,7 @@
         <v>452</v>
       </c>
       <c r="B9" s="101" t="e">
-        <f>VLOOKUP(A9,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A9,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8876,7 +8843,7 @@
         <v>452</v>
       </c>
       <c r="B10" s="101" t="e">
-        <f>VLOOKUP(A10,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A10,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8885,7 +8852,7 @@
         <v>452</v>
       </c>
       <c r="B11" s="101" t="e">
-        <f>VLOOKUP(A11,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A11,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8894,7 +8861,7 @@
         <v>452</v>
       </c>
       <c r="B12" s="101" t="e">
-        <f>VLOOKUP(A12,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A12,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8903,7 +8870,7 @@
         <v>452</v>
       </c>
       <c r="B13" s="101" t="e">
-        <f>VLOOKUP(A13,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A13,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8912,7 +8879,7 @@
         <v>452</v>
       </c>
       <c r="B14" s="101" t="e">
-        <f>VLOOKUP(A14,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A14,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8921,7 +8888,7 @@
         <v>452</v>
       </c>
       <c r="B15" s="101" t="e">
-        <f>VLOOKUP(A15,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A15,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8930,7 +8897,7 @@
         <v>452</v>
       </c>
       <c r="B16" s="101" t="e">
-        <f>VLOOKUP(A16,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A16,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8939,7 +8906,7 @@
         <v>452</v>
       </c>
       <c r="B17" s="101" t="e">
-        <f>VLOOKUP(A17,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A17,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8948,7 +8915,7 @@
         <v>452</v>
       </c>
       <c r="B18" s="101" t="e">
-        <f>VLOOKUP(A18,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A18,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8957,7 +8924,7 @@
         <v>452</v>
       </c>
       <c r="B19" s="101" t="e">
-        <f>VLOOKUP(A19,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A19,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8966,7 +8933,7 @@
         <v>452</v>
       </c>
       <c r="B20" s="101" t="e">
-        <f>VLOOKUP(A20,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A20,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8975,7 +8942,7 @@
         <v>452</v>
       </c>
       <c r="B21" s="101" t="e">
-        <f>VLOOKUP(A21,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A21,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8984,7 +8951,7 @@
         <v>452</v>
       </c>
       <c r="B22" s="101" t="e">
-        <f>VLOOKUP(A22,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A22,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -8993,7 +8960,7 @@
         <v>452</v>
       </c>
       <c r="B23" s="101" t="e">
-        <f>VLOOKUP(A23,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A23,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9002,7 +8969,7 @@
         <v>452</v>
       </c>
       <c r="B24" s="101" t="e">
-        <f>VLOOKUP(A24,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A24,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9011,7 +8978,7 @@
         <v>452</v>
       </c>
       <c r="B25" s="101" t="e">
-        <f>VLOOKUP(A25,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A25,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9020,7 +8987,7 @@
         <v>452</v>
       </c>
       <c r="B26" s="101" t="e">
-        <f>VLOOKUP(A26,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A26,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9029,7 +8996,7 @@
         <v>452</v>
       </c>
       <c r="B27" s="101" t="e">
-        <f>VLOOKUP(A27,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A27,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9038,7 +9005,7 @@
         <v>452</v>
       </c>
       <c r="B28" s="101" t="e">
-        <f>VLOOKUP(A28,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A28,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9047,7 +9014,7 @@
         <v>452</v>
       </c>
       <c r="B29" s="101" t="e">
-        <f>VLOOKUP(A29,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A29,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9056,7 +9023,7 @@
         <v>452</v>
       </c>
       <c r="B30" s="101" t="e">
-        <f>VLOOKUP(A30,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A30,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9065,7 +9032,7 @@
         <v>452</v>
       </c>
       <c r="B31" s="101" t="e">
-        <f>VLOOKUP(A31,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A31,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9074,7 +9041,7 @@
         <v>452</v>
       </c>
       <c r="B32" s="101" t="e">
-        <f>VLOOKUP(A32,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A32,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9083,7 +9050,7 @@
         <v>452</v>
       </c>
       <c r="B33" s="101" t="e">
-        <f>VLOOKUP(A33,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A33,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9092,7 +9059,7 @@
         <v>452</v>
       </c>
       <c r="B34" s="101" t="e">
-        <f>VLOOKUP(A34,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A34,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
     </row>
@@ -9101,7 +9068,7 @@
         <v>452</v>
       </c>
       <c r="B35" s="101" t="e">
-        <f>VLOOKUP(A35,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A35,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D35" s="102" t="str">
@@ -9159,7 +9126,7 @@
         <v>452</v>
       </c>
       <c r="B36" s="101" t="e">
-        <f>VLOOKUP(A36,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A36,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D36" s="103">
@@ -9229,7 +9196,7 @@
         <v>452</v>
       </c>
       <c r="B37" s="101" t="e">
-        <f>VLOOKUP(A37,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A37,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D37" s="103">
@@ -9299,7 +9266,7 @@
         <v>452</v>
       </c>
       <c r="B38" s="101" t="e">
-        <f>VLOOKUP(A38,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A38,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D38" s="103">
@@ -9369,7 +9336,7 @@
         <v>452</v>
       </c>
       <c r="B39" s="101" t="e">
-        <f>VLOOKUP(A39,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A39,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D39" s="103">
@@ -9439,7 +9406,7 @@
         <v>452</v>
       </c>
       <c r="B40" s="101" t="e">
-        <f>VLOOKUP(A40,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A40,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D40" s="103">
@@ -9509,7 +9476,7 @@
         <v>452</v>
       </c>
       <c r="B41" s="101" t="e">
-        <f>VLOOKUP(A41,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A41,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D41" s="103">
@@ -9579,7 +9546,7 @@
         <v>452</v>
       </c>
       <c r="B42" s="101" t="e">
-        <f>VLOOKUP(A42,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A42,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D42" s="103">
@@ -9649,7 +9616,7 @@
         <v>452</v>
       </c>
       <c r="B43" s="101" t="e">
-        <f>VLOOKUP(A43,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A43,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D43" s="103">
@@ -9719,7 +9686,7 @@
         <v>452</v>
       </c>
       <c r="B44" s="101" t="e">
-        <f>VLOOKUP(A44,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A44,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D44" s="103">
@@ -9789,7 +9756,7 @@
         <v>452</v>
       </c>
       <c r="B45" s="101" t="e">
-        <f>VLOOKUP(A45,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A45,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D45" s="103">
@@ -9859,7 +9826,7 @@
         <v>452</v>
       </c>
       <c r="B46" s="101" t="e">
-        <f>VLOOKUP(A46,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A46,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D46" s="103">
@@ -9929,7 +9896,7 @@
         <v>452</v>
       </c>
       <c r="B47" s="101" t="e">
-        <f>VLOOKUP(A47,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A47,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D47" s="103">
@@ -9999,7 +9966,7 @@
         <v>452</v>
       </c>
       <c r="B48" s="101" t="e">
-        <f>VLOOKUP(A48,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A48,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D48" s="103">
@@ -10069,7 +10036,7 @@
         <v>452</v>
       </c>
       <c r="B49" s="101" t="e">
-        <f>VLOOKUP(A49,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A49,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D49" s="103">
@@ -10139,7 +10106,7 @@
         <v>452</v>
       </c>
       <c r="B50" s="101" t="e">
-        <f>VLOOKUP(A50,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A50,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D50" s="103">
@@ -10209,7 +10176,7 @@
         <v>452</v>
       </c>
       <c r="B51" s="101" t="e">
-        <f>VLOOKUP(A51,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A51,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D51" s="103">
@@ -10279,7 +10246,7 @@
         <v>452</v>
       </c>
       <c r="B52" s="101" t="e">
-        <f>VLOOKUP(A52,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A52,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D52" s="103">
@@ -10349,7 +10316,7 @@
         <v>452</v>
       </c>
       <c r="B53" s="101" t="e">
-        <f>VLOOKUP(A53,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A53,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D53" s="103" t="e">
@@ -10400,7 +10367,7 @@
         <v>452</v>
       </c>
       <c r="B54" s="101" t="e">
-        <f>VLOOKUP(A54,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A54,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D54" s="103" t="e">
@@ -10451,7 +10418,7 @@
         <v>452</v>
       </c>
       <c r="B55" s="101" t="e">
-        <f>VLOOKUP(A55,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A55,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D55" s="103" t="e">
@@ -10502,7 +10469,7 @@
         <v>452</v>
       </c>
       <c r="B56" s="101" t="e">
-        <f>VLOOKUP(A56,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A56,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D56" s="103" t="e">
@@ -10553,7 +10520,7 @@
         <v>452</v>
       </c>
       <c r="B57" s="101" t="e">
-        <f>VLOOKUP(A57,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A57,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D57" s="103" t="e">
@@ -10604,7 +10571,7 @@
         <v>452</v>
       </c>
       <c r="B58" s="101" t="e">
-        <f>VLOOKUP(A58,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A58,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D58" s="103" t="e">
@@ -10655,7 +10622,7 @@
         <v>452</v>
       </c>
       <c r="B59" s="101" t="e">
-        <f>VLOOKUP(A59,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A59,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D59" s="103" t="e">
@@ -10706,7 +10673,7 @@
         <v>452</v>
       </c>
       <c r="B60" s="101" t="e">
-        <f>VLOOKUP(A60,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A60,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D60" s="103" t="e">
@@ -10757,7 +10724,7 @@
         <v>452</v>
       </c>
       <c r="B61" s="101" t="e">
-        <f>VLOOKUP(A61,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A61,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D61" s="103" t="e">
@@ -10808,7 +10775,7 @@
         <v>452</v>
       </c>
       <c r="B62" s="101" t="e">
-        <f>VLOOKUP(A62,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A62,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D62" s="103" t="e">
@@ -10859,7 +10826,7 @@
         <v>452</v>
       </c>
       <c r="B63" s="101" t="e">
-        <f>VLOOKUP(A63,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A63,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D63" s="103" t="e">
@@ -10910,7 +10877,7 @@
         <v>452</v>
       </c>
       <c r="B64" s="101" t="e">
-        <f>VLOOKUP(A64,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A64,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D64" s="103" t="e">
@@ -10961,7 +10928,7 @@
         <v>452</v>
       </c>
       <c r="B65" s="101" t="e">
-        <f>VLOOKUP(A65,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A65,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D65" s="103" t="e">
@@ -11012,7 +10979,7 @@
         <v>452</v>
       </c>
       <c r="B66" s="101" t="e">
-        <f>VLOOKUP(A66,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A66,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D66" s="103" t="e">
@@ -11063,7 +11030,7 @@
         <v>452</v>
       </c>
       <c r="B67" s="101" t="e">
-        <f>VLOOKUP(A67,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A67,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D67" s="103" t="e">
@@ -11114,7 +11081,7 @@
         <v>452</v>
       </c>
       <c r="B68" s="101" t="e">
-        <f>VLOOKUP(A68,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A68,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D68" s="103" t="e">
@@ -11165,7 +11132,7 @@
         <v>452</v>
       </c>
       <c r="B69" s="101" t="e">
-        <f>VLOOKUP(A69,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A69,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D69" s="103" t="e">
@@ -11216,7 +11183,7 @@
         <v>452</v>
       </c>
       <c r="B70" s="101" t="e">
-        <f>VLOOKUP(A70,BTP!$C$9:$C$94,1,FALSE)</f>
+        <f>VLOOKUP(A70,BTP!$C$8:$C$94,1,FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D70" s="103" t="e">

</xml_diff>